<commit_message>
added excel for traning hp sheet
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC0F5FA-E930-424E-8661-CAB5E05F7B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD8756D-DE9A-43F0-A4FA-C3FD1FEF40DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5520" yWindow="948" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>exact</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>hybrid_10_lml.csv</t>
+  </si>
+  <si>
+    <t>this one showed more values beyond lenthscale5 to train on</t>
+  </si>
+  <si>
+    <t>hybrid_10_lml_big.csv</t>
   </si>
 </sst>
 </file>
@@ -1378,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BB5A4-C3DD-4FD3-A5E3-106D216233DB}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1579,7 @@
         <v>0.5</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>50</v>
@@ -1589,34 +1595,140 @@
       </c>
       <c r="H9">
         <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>0.01</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>4.0000000000000001E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
post processing and presentation commit
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD8756D-DE9A-43F0-A4FA-C3FD1FEF40DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99FBE0F-459F-47AC-B718-908A4D401FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="948" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>exact</t>
   </si>
@@ -141,10 +141,94 @@
     <t>hybrid_10_lml.csv</t>
   </si>
   <si>
-    <t>this one showed more values beyond lenthscale5 to train on</t>
-  </si>
-  <si>
     <t>hybrid_10_lml_big.csv</t>
+  </si>
+  <si>
+    <t>exact_100_big_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_90_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_80_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_70_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_60_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_50_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_40_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_30_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_20_lml.csv</t>
+  </si>
+  <si>
+    <t>kmeans_10_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_90_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_80_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_70_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_60_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_50_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_40_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_30_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_20_lml.csv</t>
+  </si>
+  <si>
+    <t>neighbor_10_lml.csv</t>
+  </si>
+  <si>
+    <t>random_90_lml.csv</t>
+  </si>
+  <si>
+    <t>random_80_lml.csv</t>
+  </si>
+  <si>
+    <t>random_70_lml.csv</t>
+  </si>
+  <si>
+    <t>random_70_big_lml.csv</t>
+  </si>
+  <si>
+    <t>random_60_lml.csv</t>
+  </si>
+  <si>
+    <t>random_50_lml.csv</t>
+  </si>
+  <si>
+    <t>random_40_lml.csv</t>
+  </si>
+  <si>
+    <t>random_30_lml.csv</t>
+  </si>
+  <si>
+    <t>random_20_lml.csv</t>
+  </si>
+  <si>
+    <t>random_10_lml.csv</t>
   </si>
 </sst>
 </file>
@@ -205,12 +289,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,15 +1470,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BB5A4-C3DD-4FD3-A5E3-106D216233DB}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1442,60 +1528,57 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="3">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>0.5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>0.5</v>
-      </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
-      <c r="H5">
+      <c r="D5" s="3">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>0.5</v>
@@ -1521,7 +1604,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -1547,7 +1630,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>0.5</v>
@@ -1573,16 +1656,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>0.5</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>0.01</v>
@@ -1591,18 +1674,15 @@
         <v>0.5</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H9">
         <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -1628,7 +1708,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>0.5</v>
@@ -1654,79 +1734,833 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B12">
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>0.01</v>
-      </c>
-      <c r="F12">
-        <v>0.5</v>
-      </c>
-      <c r="G12">
-        <v>50</v>
-      </c>
-      <c r="H12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="B13">
         <v>0.5</v>
       </c>
       <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13">
-        <v>0.01</v>
-      </c>
-      <c r="F13">
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>50</v>
-      </c>
-      <c r="H13">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>50</v>
-      </c>
-      <c r="E14">
-        <v>0.01</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
-      </c>
-      <c r="H14">
+      <c r="B15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>50</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="3">
+        <v>50</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>0.01</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>0.01</v>
+      </c>
+      <c r="F18">
+        <v>0.5</v>
+      </c>
+      <c r="G18">
+        <v>25</v>
+      </c>
+      <c r="H18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
+      <c r="E19">
+        <v>0.01</v>
+      </c>
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>0.01</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>0.01</v>
+      </c>
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23">
+        <v>50</v>
+      </c>
+      <c r="H23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="3">
+        <v>50</v>
+      </c>
+      <c r="H24" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>0.01</v>
+      </c>
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+      <c r="G25">
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>0.01</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>0.01</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>0.01</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>25</v>
+      </c>
+      <c r="H28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <v>0.01</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+      <c r="G29">
+        <v>25</v>
+      </c>
+      <c r="H29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <v>0.5</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <v>0.01</v>
+      </c>
+      <c r="F30">
+        <v>0.75</v>
+      </c>
+      <c r="G30">
+        <v>50</v>
+      </c>
+      <c r="H30">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <v>0.01</v>
+      </c>
+      <c r="F31">
+        <v>0.75</v>
+      </c>
+      <c r="G31">
+        <v>50</v>
+      </c>
+      <c r="H31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>0.01</v>
+      </c>
+      <c r="F32">
+        <v>0.75</v>
+      </c>
+      <c r="G32">
+        <v>50</v>
+      </c>
+      <c r="H32">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3">
+        <v>70</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>70</v>
+      </c>
+      <c r="H33" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="5">
+        <v>5</v>
+      </c>
+      <c r="D34" s="5">
+        <v>25</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="5">
+        <v>25</v>
+      </c>
+      <c r="H34" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>5</v>
+      </c>
+      <c r="D35" s="5">
+        <v>25</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="5">
+        <v>25</v>
+      </c>
+      <c r="H35" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+      <c r="D36" s="5">
+        <v>25</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="5">
+        <v>25</v>
+      </c>
+      <c r="H36" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="5">
+        <v>25</v>
+      </c>
+      <c r="D37" s="5">
+        <v>50</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="5">
+        <v>50</v>
+      </c>
+      <c r="H37" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38">
+        <v>0.5</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>50</v>
+      </c>
+      <c r="E38">
+        <v>0.01</v>
+      </c>
+      <c r="F38">
+        <v>0.75</v>
+      </c>
+      <c r="G38">
+        <v>50</v>
+      </c>
+      <c r="H38">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39">
+        <v>0.5</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>0.01</v>
+      </c>
+      <c r="F39">
+        <v>0.75</v>
+      </c>
+      <c r="G39">
+        <v>50</v>
+      </c>
+      <c r="H39">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40">
+        <v>0.5</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>0.01</v>
+      </c>
+      <c r="F40">
+        <v>0.75</v>
+      </c>
+      <c r="G40">
+        <v>50</v>
+      </c>
+      <c r="H40">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41">
+        <v>0.5</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>50</v>
+      </c>
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
+        <v>0.75</v>
+      </c>
+      <c r="G41">
+        <v>50</v>
+      </c>
+      <c r="H41">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42">
+        <v>0.5</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>0.01</v>
+      </c>
+      <c r="F42">
+        <v>0.75</v>
+      </c>
+      <c r="G42">
+        <v>50</v>
+      </c>
+      <c r="H42">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="3">
+        <v>20</v>
+      </c>
+      <c r="D43" s="3">
+        <v>80</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G43" s="3">
+        <v>80</v>
+      </c>
+      <c r="H43" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
presentation, error plots, and final results
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F813870-ABA3-4203-A681-A4791B0A259F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53B3F85-8630-40EC-A74B-499DDB59E09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" activeTab="2" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="128">
   <si>
     <t>exact</t>
   </si>
@@ -277,9 +277,6 @@
     <t>kmeans_10_big_lml.csv</t>
   </si>
   <si>
-    <t>hybrid_10_lml_big2.csv</t>
-  </si>
-  <si>
     <t>neighbor_30_big_lml.csv</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
     <t>swath divisions</t>
   </si>
   <si>
-    <t>downsamle percent</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -398,14 +392,45 @@
   </si>
   <si>
     <t>Runtime</t>
+  </si>
+  <si>
+    <t>but close to the edge^</t>
+  </si>
+  <si>
+    <t>time/pcd</t>
+  </si>
+  <si>
+    <t>hybrid_10_big2_lml.csv</t>
+  </si>
+  <si>
+    <t>day 1</t>
+  </si>
+  <si>
+    <t>day 2</t>
+  </si>
+  <si>
+    <t>day2 was 92.34</t>
+  </si>
+  <si>
+    <t>looked at both plots</t>
+  </si>
+  <si>
+    <t>kinda way out there if we wanted… process noise was like 4 but didn't offer toooo much benefit so kept it smaller</t>
+  </si>
+  <si>
+    <t>kmeans was being weird when I started the script… it didn't begin processing the data until 20 seconds after running…</t>
+  </si>
+  <si>
+    <t>it also used significantly less pcds…. Fewer prediction tiles in general, is something off with the block numbers for the qeueing algo?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -432,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +473,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,24 +515,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,15 +1482,15 @@
       <c r="B22">
         <v>80</v>
       </c>
-      <c r="G22" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
+      <c r="G22" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1686,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BB5A4-C3DD-4FD3-A5E3-106D216233DB}">
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,10 +1892,10 @@
       <c r="H6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>1.06</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>0.11</v>
       </c>
       <c r="L6">
@@ -1888,10 +1936,10 @@
       <c r="H7">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>1.06</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>0.11</v>
       </c>
       <c r="L7">
@@ -1932,10 +1980,10 @@
       <c r="H8">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>1.06</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>0.11</v>
       </c>
       <c r="L8">
@@ -1976,10 +2024,10 @@
       <c r="H9">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>1.06</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>0.15</v>
       </c>
       <c r="L9">
@@ -2020,10 +2068,10 @@
       <c r="H10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>1.08</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>0.19</v>
       </c>
       <c r="L10">
@@ -2064,10 +2112,10 @@
       <c r="H11">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>1.08</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>0.23</v>
       </c>
       <c r="L11">
@@ -2108,10 +2156,10 @@
       <c r="H12">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>1.08</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="1">
         <v>0.3</v>
       </c>
       <c r="L12">
@@ -2152,31 +2200,43 @@
       <c r="H13">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="5">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14">
         <v>0.3</v>
       </c>
-      <c r="C14" s="5">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5">
-        <v>50</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>0.01</v>
+      </c>
+      <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14">
         <v>200</v>
       </c>
-      <c r="H14" s="5">
-        <v>4.0000000000000001E-3</v>
+      <c r="H14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L14">
+        <v>-19950</v>
       </c>
       <c r="R14">
         <v>0.56999999999999995</v>
@@ -2189,57 +2249,71 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="C15">
         <v>20</v>
       </c>
-      <c r="D15" s="5">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>0.01</v>
+      </c>
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" s="5">
-        <v>50</v>
-      </c>
-      <c r="H15" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16">
         <v>10</v>
       </c>
-      <c r="D16" s="5">
-        <v>50</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="5">
-        <v>50</v>
-      </c>
-      <c r="H16" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I16" s="5"/>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>0.01</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="N16">
+        <v>0.69</v>
+      </c>
+      <c r="O16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P16">
+        <v>-2840</v>
+      </c>
       <c r="R16">
         <v>1.3</v>
       </c>
@@ -2250,12 +2324,12 @@
         <v>-12520</v>
       </c>
       <c r="V16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>79</v>
+      <c r="A17" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B17" s="3">
         <v>0.3</v>
@@ -2279,9 +2353,15 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="J17" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="L17" s="3">
+        <v>-10000</v>
+      </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -2335,14 +2415,14 @@
       <c r="L18">
         <v>-120566</v>
       </c>
-      <c r="N18">
-        <v>0.69</v>
-      </c>
-      <c r="O18">
-        <v>0.18</v>
-      </c>
-      <c r="P18">
-        <v>-101817</v>
+      <c r="N18" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="P18" s="1">
+        <v>-102060</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -2379,14 +2459,14 @@
       <c r="L19">
         <v>-41320</v>
       </c>
-      <c r="N19">
-        <v>0.69</v>
-      </c>
-      <c r="O19">
-        <v>0.34</v>
-      </c>
-      <c r="P19">
-        <v>-44507</v>
+      <c r="N19" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="P19" s="1">
+        <v>-45165</v>
       </c>
       <c r="R19">
         <v>1.25</v>
@@ -2432,14 +2512,14 @@
       <c r="L20">
         <v>-58090</v>
       </c>
-      <c r="N20">
-        <v>0.69</v>
-      </c>
-      <c r="O20">
-        <v>0.34</v>
-      </c>
-      <c r="P20">
-        <v>-54450</v>
+      <c r="N20" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="P20" s="1">
+        <v>-62000</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -2476,14 +2556,14 @@
       <c r="L21">
         <v>-66578</v>
       </c>
-      <c r="N21">
-        <v>0.69</v>
-      </c>
-      <c r="O21">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="P21">
-        <v>-62980</v>
+      <c r="N21" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-66580</v>
       </c>
       <c r="R21">
         <v>1.25</v>
@@ -2529,14 +2609,14 @@
       <c r="L22">
         <v>-49160</v>
       </c>
-      <c r="N22">
-        <v>0.77</v>
-      </c>
-      <c r="O22">
-        <v>0.4</v>
-      </c>
-      <c r="P22">
-        <v>-38627</v>
+      <c r="N22" s="1">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="P22" s="1">
+        <v>-54345</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
@@ -2573,14 +2653,14 @@
       <c r="L23">
         <v>-36785</v>
       </c>
-      <c r="N23">
-        <v>0.77</v>
-      </c>
-      <c r="O23">
-        <v>0.47</v>
-      </c>
-      <c r="P23">
-        <v>-32552</v>
+      <c r="N23" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="P23" s="1">
+        <v>-43593</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
@@ -2608,6 +2688,11 @@
       <c r="H24">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="N24" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -2643,14 +2728,14 @@
       <c r="L25">
         <v>-35735</v>
       </c>
-      <c r="N25">
-        <v>0.87</v>
-      </c>
-      <c r="O25">
-        <v>0.49</v>
-      </c>
-      <c r="P25">
-        <v>-33510</v>
+      <c r="N25" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="P25" s="1">
+        <v>-36610</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -2678,6 +2763,11 @@
       <c r="H26">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="N26" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
       <c r="R26">
         <v>0.65</v>
       </c>
@@ -2722,14 +2812,14 @@
       <c r="L27">
         <v>-21551</v>
       </c>
-      <c r="N27">
-        <v>0.87</v>
-      </c>
-      <c r="O27">
-        <v>0.5</v>
-      </c>
-      <c r="P27">
-        <v>-23500</v>
+      <c r="N27" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P27" s="1">
+        <v>-17960</v>
       </c>
       <c r="R27">
         <v>1.33</v>
@@ -2766,44 +2856,60 @@
       <c r="H28">
         <v>4.0000000000000001E-3</v>
       </c>
+      <c r="N28" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="C29">
         <v>5</v>
       </c>
-      <c r="D29" s="5">
-        <v>50</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="5">
-        <v>50</v>
-      </c>
-      <c r="H29" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="10">
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29">
+        <v>0.01</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J29">
         <v>1.23</v>
       </c>
-      <c r="K29" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="L29" s="10">
+      <c r="K29">
+        <v>0.5</v>
+      </c>
+      <c r="L29">
         <v>-25832</v>
       </c>
       <c r="M29" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1.64</v>
+      </c>
+      <c r="P29" s="1">
+        <v>-17930</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
@@ -2832,13 +2938,15 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="N30" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -3128,7 +3236,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38">
         <v>0.3</v>
@@ -3195,14 +3303,14 @@
       <c r="H39">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
       <c r="R39">
         <v>1.42</v>
       </c>
@@ -3224,7 +3332,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40">
         <v>0.3</v>
@@ -3267,46 +3375,45 @@
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="B41">
+        <v>0.5</v>
+      </c>
+      <c r="C41">
         <v>10</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41">
         <v>70</v>
       </c>
-      <c r="E41" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F41" s="5">
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41">
         <v>70</v>
       </c>
-      <c r="H41" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="6">
+      <c r="H41">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41">
         <v>1.46</v>
       </c>
-      <c r="S41" s="6">
+      <c r="S41">
         <v>0.74</v>
       </c>
-      <c r="T41" s="6">
+      <c r="T41">
         <v>-25053</v>
       </c>
       <c r="V41">
@@ -3321,7 +3428,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="3">
         <v>0.5</v>
@@ -3345,13 +3452,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="9">
+      <c r="J42" s="3">
         <v>0.74</v>
       </c>
-      <c r="K42" s="9">
+      <c r="K42" s="3">
         <v>3.47</v>
       </c>
-      <c r="L42" s="9">
+      <c r="L42" s="3">
         <v>-9720</v>
       </c>
       <c r="M42" s="3"/>
@@ -3483,16 +3590,16 @@
       <c r="H45">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
       <c r="R45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.3">
@@ -3520,18 +3627,18 @@
       <c r="H46">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47">
         <v>0.5</v>
@@ -3555,7 +3662,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="J47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.3">
@@ -3715,22 +3822,22 @@
       <c r="H51">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
       <c r="S51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52">
         <v>0.3</v>
@@ -3806,19 +3913,19 @@
       <c r="H53">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54">
         <v>0.3</v>
@@ -3870,47 +3977,43 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="A55" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C55" s="5">
+      <c r="B55">
+        <v>0.5</v>
+      </c>
+      <c r="C55">
         <v>20</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55">
         <v>80</v>
       </c>
-      <c r="E55" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F55" s="5">
+      <c r="E55">
+        <v>0.01</v>
+      </c>
+      <c r="F55">
         <v>1.5</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55">
         <v>80</v>
       </c>
-      <c r="H55" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I55" s="5"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="12"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
+      <c r="H55">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="3">
         <v>0.3</v>
@@ -3944,7 +4047,7 @@
         <v>-126192</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N56" s="3">
         <v>0.69</v>
@@ -3992,10 +4095,10 @@
       <c r="H57">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="1">
         <v>1.06</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="1">
         <v>0.17599999999999999</v>
       </c>
       <c r="L57">
@@ -4009,6 +4112,15 @@
       </c>
       <c r="P57">
         <v>-54650</v>
+      </c>
+      <c r="R57" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="S57" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="T57" s="11">
+        <v>-37990</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
@@ -4036,10 +4148,10 @@
       <c r="H58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="1">
         <v>1.06</v>
       </c>
-      <c r="K58">
+      <c r="K58" s="1">
         <v>0.27</v>
       </c>
       <c r="L58">
@@ -4053,6 +4165,9 @@
       </c>
       <c r="P58">
         <v>-35272</v>
+      </c>
+      <c r="R58" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.3">
@@ -4080,10 +4195,10 @@
       <c r="H59">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="1">
         <v>1.06</v>
       </c>
-      <c r="K59">
+      <c r="K59" s="1">
         <v>0.36</v>
       </c>
       <c r="L59">
@@ -4124,18 +4239,18 @@
       <c r="H60">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B61">
         <v>0.3</v>
@@ -4158,10 +4273,10 @@
       <c r="H61">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="1">
         <v>1.07</v>
       </c>
-      <c r="K61">
+      <c r="K61" s="1">
         <v>0.62</v>
       </c>
       <c r="L61">
@@ -4187,47 +4302,42 @@
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+      <c r="A62" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C62" s="5">
+      <c r="B62">
+        <v>0.5</v>
+      </c>
+      <c r="C62">
         <v>10</v>
       </c>
-      <c r="D62" s="5">
-        <v>50</v>
-      </c>
-      <c r="E62" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F62" s="5">
+      <c r="D62">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>0.01</v>
+      </c>
+      <c r="F62">
         <v>0.75</v>
       </c>
-      <c r="G62" s="5">
-        <v>50</v>
-      </c>
-      <c r="H62" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="5"/>
-      <c r="U62" s="5"/>
+      <c r="G62">
+        <v>50</v>
+      </c>
+      <c r="H62">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="3">
         <v>0.3</v>
@@ -4251,10 +4361,10 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I63" s="3"/>
-      <c r="J63" s="3">
+      <c r="J63" s="4">
         <v>1.01</v>
       </c>
-      <c r="K63" s="3">
+      <c r="K63" s="4">
         <v>1.1200000000000001</v>
       </c>
       <c r="L63" s="3">
@@ -4301,10 +4411,10 @@
       <c r="H64">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="1">
         <v>1.08</v>
       </c>
-      <c r="K64">
+      <c r="K64" s="1">
         <v>0.16</v>
       </c>
       <c r="L64">
@@ -4345,10 +4455,10 @@
       <c r="H65">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="1">
         <v>1.08</v>
       </c>
-      <c r="K65">
+      <c r="K65" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="L65">
@@ -4389,10 +4499,10 @@
       <c r="H66">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="1">
         <v>1.08</v>
       </c>
-      <c r="K66">
+      <c r="K66" s="1">
         <v>0.39</v>
       </c>
       <c r="L66">
@@ -4433,10 +4543,10 @@
       <c r="H67">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="1">
         <v>1.08</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="1">
         <v>0.46</v>
       </c>
       <c r="L67">
@@ -4453,74 +4563,68 @@
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+      <c r="A68" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="C68" s="5">
+      <c r="B68">
+        <v>0.5</v>
+      </c>
+      <c r="C68">
         <v>10</v>
       </c>
-      <c r="D68" s="5">
-        <v>50</v>
-      </c>
-      <c r="E68" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="F68" s="5">
+      <c r="D68">
+        <v>50</v>
+      </c>
+      <c r="E68">
+        <v>0.01</v>
+      </c>
+      <c r="F68">
         <v>0.75</v>
       </c>
-      <c r="G68" s="5">
-        <v>50</v>
-      </c>
-      <c r="H68" s="5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="I68" s="5"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12"/>
-      <c r="P68" s="12"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
-      <c r="U68" s="5"/>
+      <c r="G68">
+        <v>50</v>
+      </c>
+      <c r="H68">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="9">
+      <c r="A69" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" s="3">
         <v>0.3</v>
       </c>
-      <c r="C69" s="9">
-        <v>3</v>
-      </c>
-      <c r="D69" s="9">
-        <v>50</v>
-      </c>
-      <c r="E69" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="F69" s="9">
-        <v>3</v>
-      </c>
-      <c r="G69" s="9">
+      <c r="C69" s="3">
+        <v>3</v>
+      </c>
+      <c r="D69" s="3">
+        <v>50</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F69" s="3">
+        <v>3</v>
+      </c>
+      <c r="G69" s="3">
         <v>100</v>
       </c>
-      <c r="H69" s="9">
+      <c r="H69" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I69" s="3"/>
-      <c r="J69" s="3">
+      <c r="J69" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K69" s="4">
         <v>1.6</v>
       </c>
       <c r="L69" s="3">
@@ -4550,10 +4654,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3202C004-2E8C-4251-AC07-3F29427A8F54}">
-  <dimension ref="A2:V9"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E9"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4561,402 +4666,1821 @@
     <col min="1" max="1" width="18.5546875" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" customWidth="1"/>
+    <col min="8" max="9" width="11" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" t="s">
+        <v>114</v>
+      </c>
+      <c r="V1" s="1"/>
+    </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
         <v>100</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="C2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="6">
+        <v>92.06</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="G2" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>349</v>
+      </c>
+      <c r="I2" s="15">
+        <f>E2/H2</f>
+        <v>0.26378223495702008</v>
+      </c>
+      <c r="J2" s="6">
+        <v>400</v>
+      </c>
+      <c r="K2" s="6">
+        <v>4</v>
+      </c>
+      <c r="L2" s="6">
+        <v>4</v>
+      </c>
+      <c r="M2" s="6">
+        <v>3</v>
+      </c>
+      <c r="N2" s="6">
+        <v>3</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13">
-        <v>100</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="13">
-        <v>92.06</v>
-      </c>
-      <c r="F3" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="G3" s="13">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H3" s="13">
-        <v>349</v>
-      </c>
-      <c r="I3" s="13">
+      <c r="R2" s="3">
+        <v>4</v>
+      </c>
+      <c r="T2" t="s">
+        <v>121</v>
+      </c>
+      <c r="U2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="E4" s="26">
+        <v>44.53</v>
+      </c>
+      <c r="F4">
+        <v>1.08</v>
+      </c>
+      <c r="G4">
+        <v>0.16</v>
+      </c>
+      <c r="H4">
+        <v>331</v>
+      </c>
+      <c r="I4" s="14">
+        <f>E4/H4</f>
+        <v>0.13453172205438066</v>
+      </c>
+      <c r="J4">
         <v>400</v>
       </c>
-      <c r="J3" s="13">
-        <v>4</v>
-      </c>
-      <c r="K3" s="13">
-        <v>4</v>
-      </c>
-      <c r="L3" s="13">
-        <v>3</v>
-      </c>
-      <c r="M3" s="13">
-        <v>3</v>
-      </c>
-      <c r="N3" s="13" t="s">
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>108</v>
+      </c>
+      <c r="P4" t="s">
         <v>109</v>
       </c>
-      <c r="O3" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8">
+        <v>6.83E-2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="E5" s="26">
+        <v>28.54</v>
+      </c>
+      <c r="F5">
+        <v>1.08</v>
+      </c>
+      <c r="G5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H5">
+        <v>322</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" ref="I5:I31" si="0">E5/H5</f>
+        <v>8.8633540372670808E-2</v>
+      </c>
+      <c r="J5">
+        <v>400</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
         <v>108</v>
       </c>
-      <c r="Q3" s="3">
-        <v>4</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="P5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5">
-        <v>50</v>
-      </c>
-      <c r="C5" s="15">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D5" s="15">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="E5" s="6">
-        <v>44.53</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="T5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E6" s="26">
+        <v>22.69</v>
+      </c>
+      <c r="F6">
         <v>1.08</v>
       </c>
-      <c r="G5" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="H5" s="6">
-        <v>331</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="G6">
+        <v>0.39</v>
+      </c>
+      <c r="H6">
+        <v>313</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>7.2492012779552722E-2</v>
+      </c>
+      <c r="J6">
         <v>400</v>
       </c>
-      <c r="J5" s="5">
-        <v>4</v>
-      </c>
-      <c r="K5" s="5">
-        <v>4</v>
-      </c>
-      <c r="L5" s="5">
-        <v>3</v>
-      </c>
-      <c r="M5" s="5">
-        <v>3</v>
-      </c>
-      <c r="N5" s="5" t="s">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>108</v>
+      </c>
+      <c r="P6" t="s">
         <v>109</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P5" s="5" t="s">
+      <c r="Q6" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>0.5</v>
-      </c>
-      <c r="T5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="T6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.1047</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="E7" s="26">
+        <v>18.71</v>
+      </c>
+      <c r="F7">
+        <v>1.08</v>
+      </c>
+      <c r="G7">
+        <v>0.46</v>
+      </c>
+      <c r="H7">
+        <v>304</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>6.1546052631578953E-2</v>
+      </c>
+      <c r="J7">
+        <v>400</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="T7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.1663</v>
+      </c>
+      <c r="D8" s="9">
+        <v>9.5299999999999996E-2</v>
+      </c>
+      <c r="E8" s="27">
+        <v>10.74</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="H8" s="3">
+        <v>229</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="0"/>
+        <v>4.6899563318777295E-2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>400</v>
+      </c>
+      <c r="K8" s="3">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
+        <v>4</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3</v>
+      </c>
+      <c r="N8" s="3">
+        <v>3</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="3">
+        <v>4</v>
+      </c>
+      <c r="T8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11">
+        <v>50</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5.6399999999999999E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="E9" s="28">
+        <v>43.43</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="H9" s="16">
+        <v>338</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.12849112426035503</v>
+      </c>
+      <c r="J9">
+        <v>400</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="T9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11">
         <v>33</v>
       </c>
-      <c r="C6" s="15">
-        <v>6.83E-2</v>
-      </c>
-      <c r="D6" s="15">
-        <v>4.1200000000000001E-2</v>
-      </c>
-      <c r="E6" s="6">
-        <v>28.54</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="C10" s="18">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="E10" s="28">
+        <v>30.45</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0.27</v>
+      </c>
+      <c r="H10" s="12">
+        <v>326</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="0"/>
+        <v>9.3404907975460125E-2</v>
+      </c>
+      <c r="J10">
+        <v>400</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="T10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="11">
+        <v>25</v>
+      </c>
+      <c r="C11" s="18">
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="E11" s="28">
+        <v>23.47</v>
+      </c>
+      <c r="F11" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.36</v>
+      </c>
+      <c r="H11" s="12">
+        <v>313</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="0"/>
+        <v>7.4984025559105424E-2</v>
+      </c>
+      <c r="J11">
+        <v>400</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>108</v>
+      </c>
+      <c r="P11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="T11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11">
+        <v>20</v>
+      </c>
+      <c r="C12" s="18">
+        <v>8.7400000000000005E-2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="E12" s="28">
+        <v>19.18</v>
+      </c>
+      <c r="F12" s="12">
+        <v>1.07</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0.62</v>
+      </c>
+      <c r="H12" s="12">
+        <v>306</v>
+      </c>
+      <c r="I12" s="14">
+        <f t="shared" si="0"/>
+        <v>6.2679738562091497E-2</v>
+      </c>
+      <c r="J12">
+        <v>400</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>108</v>
+      </c>
+      <c r="P12" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="T12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="19">
+        <v>10</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0.21340000000000001</v>
+      </c>
+      <c r="D13" s="20">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="E13" s="29">
+        <v>11.16</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1.01</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H13" s="21">
+        <v>252</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="0"/>
+        <v>4.4285714285714289E-2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>400</v>
+      </c>
+      <c r="K13" s="3">
+        <v>4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>4</v>
+      </c>
+      <c r="M13" s="3">
+        <v>3</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="3">
+        <v>4</v>
+      </c>
+      <c r="T13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>90</v>
+      </c>
+      <c r="C14" s="18">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="D14" s="18">
+        <v>5.2200000000000003E-2</v>
+      </c>
+      <c r="E14" s="28">
+        <v>110.15</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="H14" s="16">
+        <v>296</v>
+      </c>
+      <c r="I14" s="24">
+        <f t="shared" si="0"/>
+        <v>0.37212837837837842</v>
+      </c>
+      <c r="J14">
+        <v>400</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>108</v>
+      </c>
+      <c r="P14" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="T14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11">
+        <v>80</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.1047</v>
+      </c>
+      <c r="D15" s="18">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="E15" s="28">
+        <v>89.53</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G15" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="H15" s="16">
+        <v>290</v>
+      </c>
+      <c r="I15" s="24">
+        <f t="shared" si="0"/>
+        <v>0.30872413793103448</v>
+      </c>
+      <c r="J15">
+        <v>400</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="T15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>70</v>
+      </c>
+      <c r="C16" s="18">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>4.36E-2</v>
+      </c>
+      <c r="E16" s="28">
+        <v>73.28</v>
+      </c>
+      <c r="F16" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="H16" s="16">
+        <v>299</v>
+      </c>
+      <c r="I16" s="24">
+        <f t="shared" si="0"/>
+        <v>0.24508361204013379</v>
+      </c>
+      <c r="J16">
+        <v>400</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>108</v>
+      </c>
+      <c r="P16" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="T16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11">
+        <v>60</v>
+      </c>
+      <c r="C17" s="18">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="D17" s="18">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="E17" s="28">
+        <v>65.94</v>
+      </c>
+      <c r="F17" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="H17" s="16">
+        <v>291</v>
+      </c>
+      <c r="I17" s="24">
+        <f t="shared" si="0"/>
+        <v>0.22659793814432988</v>
+      </c>
+      <c r="J17">
+        <v>400</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+      <c r="O17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P17" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>13</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="T17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="11">
+        <v>50</v>
+      </c>
+      <c r="C18" s="18">
+        <v>9.7900000000000001E-2</v>
+      </c>
+      <c r="D18" s="18">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="E18" s="28">
+        <v>54.77</v>
+      </c>
+      <c r="F18" s="12">
         <v>1.08</v>
       </c>
-      <c r="G6" s="5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H6" s="6">
-        <v>322</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="G18" s="12">
+        <v>0.19</v>
+      </c>
+      <c r="H18" s="16">
+        <v>271</v>
+      </c>
+      <c r="I18" s="24">
+        <f t="shared" si="0"/>
+        <v>0.20210332103321035</v>
+      </c>
+      <c r="J18">
         <v>400</v>
       </c>
-      <c r="J6" s="5">
-        <v>4</v>
-      </c>
-      <c r="K6" s="5">
-        <v>4</v>
-      </c>
-      <c r="L6" s="5">
-        <v>3</v>
-      </c>
-      <c r="M6" s="5">
-        <v>3</v>
-      </c>
-      <c r="N6" s="5" t="s">
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P18" t="s">
         <v>109</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>4</v>
-      </c>
-      <c r="R6">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5">
-        <v>25</v>
-      </c>
-      <c r="C7" s="15">
-        <v>8.4699999999999998E-2</v>
-      </c>
-      <c r="D7" s="15">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>22.69</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="Q18" t="s">
+        <v>13</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="T18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="11">
+        <v>40</v>
+      </c>
+      <c r="C19" s="18">
+        <v>9.64E-2</v>
+      </c>
+      <c r="D19" s="18">
+        <v>5.8599999999999999E-2</v>
+      </c>
+      <c r="E19" s="28">
+        <v>43.44</v>
+      </c>
+      <c r="F19" s="12">
         <v>1.08</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G19" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="H19" s="16">
+        <v>270</v>
+      </c>
+      <c r="I19" s="24">
+        <f t="shared" si="0"/>
+        <v>0.16088888888888889</v>
+      </c>
+      <c r="J19">
+        <v>400</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P19" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>13</v>
+      </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
+      <c r="T19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="11">
+        <v>30</v>
+      </c>
+      <c r="C20" s="18">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="D20" s="18">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="E20" s="28">
+        <v>30.46</v>
+      </c>
+      <c r="F20" s="12">
+        <v>1.08</v>
+      </c>
+      <c r="G20" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H20" s="12">
+        <v>277</v>
+      </c>
+      <c r="I20" s="24">
+        <f t="shared" si="0"/>
+        <v>0.10996389891696751</v>
+      </c>
+      <c r="J20">
+        <v>400</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
+        <v>108</v>
+      </c>
+      <c r="P20" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+      <c r="T20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="11">
+        <v>20</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.1162</v>
+      </c>
+      <c r="D21" s="18">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="E21" s="28">
+        <v>20.5</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1.08</v>
+      </c>
+      <c r="G21" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="12">
+        <v>247</v>
+      </c>
+      <c r="I21" s="24">
+        <f t="shared" si="0"/>
+        <v>8.2995951417004055E-2</v>
+      </c>
+      <c r="J21">
+        <v>400</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>108</v>
+      </c>
+      <c r="P21" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
+      </c>
+      <c r="T21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="19">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.16589999999999999</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.1009</v>
+      </c>
+      <c r="E22" s="27">
+        <v>10.83</v>
+      </c>
+      <c r="F22" s="13">
+        <v>1.18</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.62</v>
+      </c>
+      <c r="H22" s="21">
+        <v>195</v>
+      </c>
+      <c r="I22" s="25">
+        <f t="shared" si="0"/>
+        <v>5.5538461538461537E-2</v>
+      </c>
+      <c r="J22" s="3">
+        <v>400</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3">
+        <v>4</v>
+      </c>
+      <c r="M22" s="3">
+        <v>3</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R22" s="3">
+        <v>4</v>
+      </c>
+      <c r="T22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="11">
+        <v>90</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0.12809999999999999</v>
+      </c>
+      <c r="D23" s="18">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="E23" s="28">
+        <v>150.76</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.88</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="H23" s="16">
+        <v>176</v>
+      </c>
+      <c r="I23" s="24">
+        <f t="shared" si="0"/>
+        <v>0.85659090909090907</v>
+      </c>
+      <c r="J23">
+        <v>400</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23" t="s">
+        <v>108</v>
+      </c>
+      <c r="P23" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>17</v>
+      </c>
+      <c r="R23" s="11">
+        <v>4</v>
+      </c>
+      <c r="T23" t="s">
+        <v>122</v>
+      </c>
+      <c r="U23" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="11">
+        <v>80</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.1085</v>
+      </c>
+      <c r="D24" s="18">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="E24" s="28">
+        <v>125.29</v>
+      </c>
+      <c r="F24" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H24" s="16">
+        <v>176</v>
+      </c>
+      <c r="I24" s="24">
+        <f t="shared" si="0"/>
+        <v>0.71187500000000004</v>
+      </c>
+      <c r="J24">
+        <v>400</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24" t="s">
+        <v>108</v>
+      </c>
+      <c r="P24" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>17</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="T24" t="s">
+        <v>122</v>
+      </c>
+      <c r="U24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="11">
+        <v>70</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0.11269999999999999</v>
+      </c>
+      <c r="D25" s="18">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="E25" s="28">
+        <v>103.57</v>
+      </c>
+      <c r="F25" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H25" s="16">
+        <v>171</v>
+      </c>
+      <c r="I25" s="24">
+        <f t="shared" si="0"/>
+        <v>0.60567251461988303</v>
+      </c>
+      <c r="J25">
+        <v>400</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25" t="s">
+        <v>108</v>
+      </c>
+      <c r="P25" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>17</v>
+      </c>
+      <c r="R25">
+        <v>4</v>
+      </c>
+      <c r="T25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="11">
+        <v>60</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.12429999999999999</v>
+      </c>
+      <c r="D26" s="18">
+        <v>7.0900000000000005E-2</v>
+      </c>
+      <c r="E26" s="28">
+        <v>82.77</v>
+      </c>
+      <c r="F26" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="H26" s="16">
+        <v>175</v>
+      </c>
+      <c r="I26" s="24">
+        <f t="shared" si="0"/>
+        <v>0.47297142857142854</v>
+      </c>
+      <c r="J26">
+        <v>400</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+      <c r="O26" t="s">
+        <v>108</v>
+      </c>
+      <c r="P26" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>17</v>
+      </c>
+      <c r="R26">
+        <v>4</v>
+      </c>
+      <c r="T26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="11">
+        <v>50</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0.1111</v>
+      </c>
+      <c r="D27" s="18">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="E27" s="28">
+        <v>67.3</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0.19</v>
+      </c>
+      <c r="H27" s="16">
+        <v>172</v>
+      </c>
+      <c r="I27" s="24">
+        <f t="shared" si="0"/>
+        <v>0.39127906976744187</v>
+      </c>
+      <c r="J27">
+        <v>400</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27" t="s">
+        <v>108</v>
+      </c>
+      <c r="P27" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>17</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="T27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="11">
+        <v>40</v>
+      </c>
+      <c r="C28" s="18">
+        <v>9.4899999999999998E-2</v>
+      </c>
+      <c r="D28" s="18">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="E28" s="28">
+        <v>49.68</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1.23</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0.22</v>
+      </c>
+      <c r="H28" s="16">
+        <v>163</v>
+      </c>
+      <c r="I28" s="24">
+        <f t="shared" si="0"/>
+        <v>0.3047852760736196</v>
+      </c>
+      <c r="J28">
+        <v>400</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28" t="s">
+        <v>108</v>
+      </c>
+      <c r="P28" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>17</v>
+      </c>
+      <c r="R28">
+        <v>4</v>
+      </c>
+      <c r="T28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="11">
+        <v>30</v>
+      </c>
+      <c r="C29" s="18">
+        <v>0.106</v>
+      </c>
+      <c r="D29" s="18">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="E29" s="28">
+        <v>35.69</v>
+      </c>
+      <c r="F29" s="12">
+        <v>1.05</v>
+      </c>
+      <c r="G29" s="12">
         <v>0.39</v>
       </c>
-      <c r="H7" s="6">
-        <v>313</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="H29" s="16">
+        <v>166</v>
+      </c>
+      <c r="I29" s="24">
+        <f t="shared" si="0"/>
+        <v>0.215</v>
+      </c>
+      <c r="J29">
         <v>400</v>
       </c>
-      <c r="J7" s="5">
-        <v>4</v>
-      </c>
-      <c r="K7" s="5">
-        <v>4</v>
-      </c>
-      <c r="L7" s="5">
-        <v>3</v>
-      </c>
-      <c r="M7" s="5">
-        <v>3</v>
-      </c>
-      <c r="N7" s="5" t="s">
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29" t="s">
+        <v>108</v>
+      </c>
+      <c r="P29" t="s">
         <v>109</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="Q29" t="s">
+        <v>17</v>
+      </c>
+      <c r="R29">
+        <v>4</v>
+      </c>
+      <c r="T29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="11">
         <v>20</v>
       </c>
-      <c r="C8" s="15">
-        <v>0.1047</v>
-      </c>
-      <c r="D8" s="15">
-        <v>5.3100000000000001E-2</v>
-      </c>
-      <c r="E8" s="6">
-        <v>18.71</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1.08</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.46</v>
-      </c>
-      <c r="H8" s="6">
-        <v>304</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="C30" s="18">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="D30" s="18">
+        <v>6.2600000000000003E-2</v>
+      </c>
+      <c r="E30" s="28">
+        <v>21.34</v>
+      </c>
+      <c r="F30" s="12">
+        <v>1.01</v>
+      </c>
+      <c r="G30" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="H30" s="16">
+        <v>161</v>
+      </c>
+      <c r="I30" s="24">
+        <f t="shared" si="0"/>
+        <v>0.13254658385093168</v>
+      </c>
+      <c r="J30">
         <v>400</v>
       </c>
-      <c r="J8" s="5">
-        <v>4</v>
-      </c>
-      <c r="K8" s="5">
-        <v>4</v>
-      </c>
-      <c r="L8" s="5">
-        <v>3</v>
-      </c>
-      <c r="M8" s="5">
-        <v>3</v>
-      </c>
-      <c r="N8" s="5" t="s">
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>3</v>
+      </c>
+      <c r="O30" t="s">
+        <v>108</v>
+      </c>
+      <c r="P30" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="Q30" t="s">
+        <v>17</v>
+      </c>
+      <c r="R30">
+        <v>4</v>
+      </c>
+      <c r="T30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="19">
         <v>10</v>
       </c>
-      <c r="C9" s="16">
-        <v>0.1663</v>
-      </c>
-      <c r="D9" s="16">
-        <v>9.5299999999999996E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>10.74</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="H9" s="3">
-        <v>229</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="C31" s="3">
+        <v>0.15129999999999999</v>
+      </c>
+      <c r="D31" s="3">
+        <v>9.3899999999999997E-2</v>
+      </c>
+      <c r="E31" s="29">
+        <v>10.29</v>
+      </c>
+      <c r="F31" s="13">
+        <v>1.01</v>
+      </c>
+      <c r="G31" s="13">
+        <v>1.64</v>
+      </c>
+      <c r="H31" s="21">
+        <v>139</v>
+      </c>
+      <c r="I31" s="25">
+        <f t="shared" si="0"/>
+        <v>7.4028776978417254E-2</v>
+      </c>
+      <c r="J31" s="3">
         <v>400</v>
       </c>
-      <c r="J9" s="3">
-        <v>4</v>
-      </c>
-      <c r="K9" s="3">
-        <v>4</v>
-      </c>
-      <c r="L9" s="3">
-        <v>3</v>
-      </c>
-      <c r="M9" s="3">
-        <v>3</v>
-      </c>
-      <c r="N9" s="3" t="s">
+      <c r="K31" s="3">
+        <v>4</v>
+      </c>
+      <c r="L31" s="3">
+        <v>4</v>
+      </c>
+      <c r="M31" s="3">
+        <v>3</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P31" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>4</v>
-      </c>
-      <c r="R9" s="3"/>
+      <c r="Q31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R31" s="3">
+        <v>4</v>
+      </c>
+      <c r="T31" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor updates and trainig
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53B3F85-8630-40EC-A74B-499DDB59E09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DC29B5-F4E3-4387-9D0E-AF5E91ABEC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="130">
   <si>
     <t>exact</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>it also used significantly less pcds…. Fewer prediction tiles in general, is something off with the block numbers for the qeueing algo?</t>
+  </si>
+  <si>
+    <t>didn't want to jack up the process noise</t>
+  </si>
+  <si>
+    <t>may need to rerun if 70 doesn't converge, watch sparsity closesly</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -457,7 +463,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +485,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -527,29 +545,32 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1732,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515BB5A4-C3DD-4FD3-A5E3-106D216233DB}">
-  <dimension ref="A1:X69"/>
+  <dimension ref="A1:AF69"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18:O30"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2200,9 +2221,9 @@
       <c r="H13">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -2273,9 +2294,9 @@
       <c r="H15">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2302,9 +2323,9 @@
       <c r="H16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
       <c r="N16">
         <v>0.69</v>
       </c>
@@ -2688,11 +2709,11 @@
       <c r="H24">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -2763,11 +2784,11 @@
       <c r="H26">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N26" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
       <c r="R26">
         <v>0.65</v>
       </c>
@@ -2856,11 +2877,11 @@
       <c r="H28">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N28" s="23" t="s">
+      <c r="N28" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2942,11 +2963,11 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
@@ -2978,13 +2999,22 @@
       <c r="H31">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="L31">
+        <v>-89370</v>
+      </c>
+      <c r="N31">
         <v>1.06</v>
       </c>
-      <c r="K31">
+      <c r="O31">
         <v>0.09</v>
       </c>
-      <c r="L31">
+      <c r="P31">
         <v>-94635</v>
       </c>
     </row>
@@ -3013,17 +3043,26 @@
       <c r="H32">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="L32">
+        <v>-99030</v>
+      </c>
+      <c r="N32">
         <v>1.25</v>
       </c>
-      <c r="K32">
+      <c r="O32">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L32">
+      <c r="P32">
         <v>-109572</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3048,17 +3087,26 @@
       <c r="H33">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="L33">
+        <v>-86730</v>
+      </c>
+      <c r="N33">
         <v>1.25</v>
       </c>
-      <c r="K33">
+      <c r="O33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L33">
+      <c r="P33">
         <v>-109572</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -3083,26 +3131,44 @@
       <c r="H34">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="L34">
+        <v>-65120</v>
+      </c>
+      <c r="N34">
         <v>1.44</v>
       </c>
-      <c r="K34">
+      <c r="O34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L34">
+      <c r="P34">
         <v>-83349</v>
       </c>
-      <c r="N34">
+      <c r="R34">
         <v>1.06</v>
       </c>
-      <c r="O34">
+      <c r="S34">
         <v>0.13</v>
       </c>
-      <c r="P34">
+      <c r="T34">
         <v>-65116</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z34">
+        <v>1.06</v>
+      </c>
+      <c r="AA34">
+        <v>0.13</v>
+      </c>
+      <c r="AB34">
+        <v>-65116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -3127,26 +3193,44 @@
       <c r="H35">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="L35">
+        <v>-41760</v>
+      </c>
+      <c r="N35">
         <v>1.44</v>
       </c>
-      <c r="K35">
+      <c r="O35">
         <v>0.15</v>
       </c>
-      <c r="L35">
+      <c r="P35">
         <v>-48002</v>
       </c>
-      <c r="N35">
+      <c r="R35">
         <v>1.06</v>
       </c>
-      <c r="O35">
+      <c r="S35">
         <v>0.19</v>
       </c>
-      <c r="P35">
+      <c r="T35">
         <v>-44941</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z35">
+        <v>1.06</v>
+      </c>
+      <c r="AA35">
+        <v>0.19</v>
+      </c>
+      <c r="AB35">
+        <v>-44941</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -3171,26 +3255,44 @@
       <c r="H36">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="L36">
+        <v>-34000</v>
+      </c>
+      <c r="N36">
         <v>1.42</v>
       </c>
-      <c r="K36">
+      <c r="O36">
         <v>0.22</v>
       </c>
-      <c r="L36">
+      <c r="P36">
         <v>-45277</v>
       </c>
-      <c r="N36">
+      <c r="R36">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O36">
+      <c r="S36">
         <v>0.21</v>
       </c>
-      <c r="P36">
+      <c r="T36">
         <v>-43136</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z36">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AA36">
+        <v>0.21</v>
+      </c>
+      <c r="AB36">
+        <v>-43136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -3215,26 +3317,44 @@
       <c r="H37">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="L37">
+        <v>-28390</v>
+      </c>
+      <c r="N37">
         <v>1.42</v>
       </c>
-      <c r="K37">
+      <c r="O37">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L37">
+      <c r="P37">
         <v>-35391</v>
       </c>
-      <c r="N37">
+      <c r="R37">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O37">
+      <c r="S37">
         <v>0.39</v>
       </c>
-      <c r="P37">
+      <c r="T37">
         <v>-27238</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Z37">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AA37">
+        <v>0.39</v>
+      </c>
+      <c r="AB37">
+        <v>-27238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -3259,26 +3379,41 @@
       <c r="H38">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="K38" s="25"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38">
         <v>0.96</v>
       </c>
-      <c r="K38">
+      <c r="O38">
         <v>0.52</v>
       </c>
-      <c r="L38">
+      <c r="P38">
         <v>-23150</v>
       </c>
-      <c r="R38">
+      <c r="V38">
         <v>0.47</v>
       </c>
-      <c r="S38">
+      <c r="W38">
         <v>3.47</v>
       </c>
-      <c r="T38">
+      <c r="X38">
         <v>-14240</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AD38">
+        <v>0.47</v>
+      </c>
+      <c r="AE38">
+        <v>3.47</v>
+      </c>
+      <c r="AF38">
+        <v>-14240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -3303,34 +3438,49 @@
       <c r="H39">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
+      <c r="J39" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="L39">
+        <v>-22240</v>
+      </c>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
-      <c r="R39">
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39">
         <v>1.42</v>
       </c>
-      <c r="S39">
+      <c r="W39">
         <v>0.34</v>
       </c>
-      <c r="T39">
+      <c r="X39">
         <v>-25976</v>
       </c>
-      <c r="V39">
-        <v>0.96</v>
-      </c>
-      <c r="W39">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="X39">
-        <v>-19837</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39">
+        <v>1.42</v>
+      </c>
+      <c r="AE39">
+        <v>0.34</v>
+      </c>
+      <c r="AF39">
+        <v>-25976</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -3355,26 +3505,41 @@
       <c r="H40">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="K40" s="25"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40">
         <v>1.02</v>
       </c>
-      <c r="K40">
+      <c r="O40">
         <v>0.72</v>
       </c>
-      <c r="L40">
+      <c r="P40">
         <v>-16952</v>
       </c>
-      <c r="R40">
+      <c r="V40">
         <v>0.52</v>
       </c>
-      <c r="S40">
+      <c r="W40">
         <v>3.68</v>
       </c>
-      <c r="T40">
+      <c r="X40">
         <v>-11770</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AD40">
+        <v>0.52</v>
+      </c>
+      <c r="AE40">
+        <v>3.68</v>
+      </c>
+      <c r="AF40">
+        <v>-11770</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -3399,34 +3564,49 @@
       <c r="H41">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
+      <c r="J41" s="26">
+        <v>0.96</v>
+      </c>
+      <c r="K41" s="26">
+        <v>0.71</v>
+      </c>
+      <c r="L41" s="23">
+        <v>-20950</v>
+      </c>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
-      <c r="R41">
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41">
         <v>1.46</v>
       </c>
-      <c r="S41">
+      <c r="W41">
         <v>0.74</v>
       </c>
-      <c r="T41">
+      <c r="X41">
         <v>-25053</v>
       </c>
-      <c r="V41">
-        <v>0.91</v>
-      </c>
-      <c r="W41">
-        <v>0.94</v>
-      </c>
-      <c r="X41">
-        <v>-18007</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="5"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41">
+        <v>1.46</v>
+      </c>
+      <c r="AE41">
+        <v>0.74</v>
+      </c>
+      <c r="AF41">
+        <v>-25053</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>81</v>
       </c>
@@ -3452,32 +3632,51 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="3">
+      <c r="J42" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="K42" s="27"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="3">
         <v>0.74</v>
       </c>
-      <c r="K42" s="3">
+      <c r="O42" s="3">
         <v>3.47</v>
       </c>
-      <c r="L42" s="3">
+      <c r="P42" s="3">
         <v>-9720</v>
       </c>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
-      <c r="R42" s="3">
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3">
         <v>0.96</v>
       </c>
-      <c r="S42" s="3">
+      <c r="W42" s="3">
         <v>3.68</v>
       </c>
-      <c r="T42" s="3">
+      <c r="X42" s="3">
         <v>-10720</v>
       </c>
-      <c r="U42" s="3"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="AE42" s="3">
+        <v>3.68</v>
+      </c>
+      <c r="AF42" s="3">
+        <v>-10720</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -3502,26 +3701,35 @@
       <c r="H43">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="1">
         <v>1.06</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="1">
         <v>0.09</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
+        <v>-104180</v>
+      </c>
+      <c r="R43">
+        <v>1.06</v>
+      </c>
+      <c r="S43">
+        <v>0.09</v>
+      </c>
+      <c r="T43">
         <v>-104176</v>
       </c>
-      <c r="N43">
+      <c r="V43">
         <v>0.69</v>
       </c>
-      <c r="O43">
+      <c r="W43">
         <v>0.17</v>
       </c>
-      <c r="P43">
+      <c r="X43">
         <v>-92757</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -3546,26 +3754,35 @@
       <c r="H44">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="1">
         <v>1.06</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="1">
         <v>0.11</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1">
+        <v>-88420</v>
+      </c>
+      <c r="R44">
+        <v>1.06</v>
+      </c>
+      <c r="S44">
+        <v>0.11</v>
+      </c>
+      <c r="T44">
         <v>-88422</v>
       </c>
-      <c r="N44">
+      <c r="V44">
         <v>0.69</v>
       </c>
-      <c r="O44">
+      <c r="W44">
         <v>0.24</v>
       </c>
-      <c r="P44">
+      <c r="X44">
         <v>-76100</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -3590,19 +3807,28 @@
       <c r="H45">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" t="s">
+      <c r="J45" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L45" s="1">
+        <v>-78730</v>
+      </c>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -3627,16 +3853,21 @@
       <c r="H46">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J46" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -3661,11 +3892,14 @@
       <c r="H47">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="R47" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3690,26 +3924,35 @@
       <c r="H48">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L48" s="1">
+        <v>-66300</v>
+      </c>
+      <c r="R48">
         <v>1.08</v>
       </c>
-      <c r="K48">
+      <c r="S48">
         <v>0.16</v>
       </c>
-      <c r="L48">
+      <c r="T48">
         <v>-62166</v>
       </c>
-      <c r="N48">
+      <c r="V48">
         <v>0.69</v>
       </c>
-      <c r="O48">
+      <c r="W48">
         <v>0.27</v>
       </c>
-      <c r="P48">
+      <c r="X48">
         <v>-59638</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -3734,26 +3977,35 @@
       <c r="H49">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="L49" s="1">
+        <v>-53290</v>
+      </c>
+      <c r="R49">
         <v>1.08</v>
       </c>
-      <c r="K49">
+      <c r="S49">
         <v>0.18</v>
       </c>
-      <c r="L49">
+      <c r="T49">
         <v>-59682</v>
       </c>
-      <c r="N49">
+      <c r="V49">
         <v>0.69</v>
       </c>
-      <c r="O49">
+      <c r="W49">
         <v>0.34</v>
       </c>
-      <c r="P49">
+      <c r="X49">
         <v>-46780</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3778,26 +4030,35 @@
       <c r="H50">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="L50" s="1">
+        <v>-42050</v>
+      </c>
+      <c r="R50">
         <v>1.08</v>
       </c>
-      <c r="K50">
+      <c r="S50">
         <v>0.24</v>
       </c>
-      <c r="L50">
+      <c r="T50">
         <v>-42050</v>
       </c>
-      <c r="N50">
+      <c r="V50">
         <v>0.69</v>
       </c>
-      <c r="O50">
+      <c r="W50">
         <v>0.43</v>
       </c>
-      <c r="P50">
+      <c r="X50">
         <v>-36400</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3822,20 +4083,29 @@
       <c r="H51">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
+      <c r="J51" s="1">
+        <v>1.27</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L51" s="1">
+        <v>-35950</v>
+      </c>
       <c r="R51" s="5"/>
-      <c r="S51" t="s">
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -3860,35 +4130,38 @@
       <c r="H52">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="R52">
         <v>1.07</v>
       </c>
-      <c r="K52">
+      <c r="S52">
         <v>0.34</v>
       </c>
-      <c r="L52">
+      <c r="T52">
         <v>-33072</v>
       </c>
-      <c r="N52">
+      <c r="V52">
         <v>0.69</v>
       </c>
-      <c r="O52">
+      <c r="W52">
         <v>1.07</v>
       </c>
-      <c r="P52">
+      <c r="X52">
         <v>-20117</v>
       </c>
-      <c r="R52">
+      <c r="Z52">
         <v>0.46</v>
       </c>
-      <c r="S52">
+      <c r="AA52">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T52">
+      <c r="AB52">
         <v>-12370</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3913,17 +4186,26 @@
       <c r="H53">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
+      <c r="J53" s="1">
+        <v>1.27</v>
+      </c>
+      <c r="K53" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="L53" s="1">
+        <v>-22000</v>
+      </c>
       <c r="R53" s="5"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -3948,35 +4230,38 @@
       <c r="H54">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="R54">
         <v>1.07</v>
       </c>
-      <c r="K54">
+      <c r="S54">
         <v>0.57999999999999996</v>
       </c>
-      <c r="L54">
+      <c r="T54">
         <v>-19230</v>
       </c>
-      <c r="N54">
+      <c r="V54">
         <v>0.69</v>
       </c>
-      <c r="O54">
+      <c r="W54">
         <v>3.19</v>
       </c>
-      <c r="P54">
+      <c r="X54">
         <v>-9953</v>
       </c>
-      <c r="R54">
+      <c r="Z54">
         <v>0.63</v>
       </c>
-      <c r="S54">
+      <c r="AA54">
         <v>6.2</v>
       </c>
-      <c r="T54">
+      <c r="AB54">
         <v>-8914</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -4001,17 +4286,26 @@
       <c r="H55">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
+      <c r="J55" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="K55" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L55" s="1">
+        <v>-15070</v>
+      </c>
       <c r="R55" s="5"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>84</v>
       </c>
@@ -4037,40 +4331,48 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="3">
-        <v>1.07</v>
-      </c>
-      <c r="K56" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L56" s="3">
-        <v>-126192</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N56" s="3">
-        <v>0.69</v>
-      </c>
-      <c r="O56" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="P56" s="3">
-        <v>-67030</v>
-      </c>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="S56" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T56" s="3">
+        <v>-126192</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V56" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="W56" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="X56" s="3">
+        <v>-67030</v>
+      </c>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3">
         <v>0.36</v>
       </c>
-      <c r="S56" s="3">
+      <c r="AA56" s="3">
         <v>0.68</v>
       </c>
-      <c r="T56" s="3">
+      <c r="AB56" s="3">
         <v>-73685</v>
       </c>
-      <c r="U56" s="3"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="AC56" s="3"/>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -4116,14 +4418,14 @@
       <c r="R57" s="5">
         <v>0.86</v>
       </c>
-      <c r="S57" s="11">
+      <c r="S57">
         <v>0.33</v>
       </c>
-      <c r="T57" s="11">
+      <c r="T57">
         <v>-37990</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -4170,7 +4472,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -4214,7 +4516,7 @@
         <v>-27490</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -4248,7 +4550,7 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -4301,7 +4603,7 @@
         <v>-11700</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -4335,7 +4637,7 @@
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>88</v>
       </c>
@@ -4386,7 +4688,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -4654,11 +4956,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3202C004-2E8C-4251-AC07-3F29427A8F54}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O33" sqref="O33"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4756,11 +5058,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H2" s="6">
-        <v>349</v>
-      </c>
-      <c r="I2" s="15">
+        <v>350</v>
+      </c>
+      <c r="I2" s="12">
         <f>E2/H2</f>
-        <v>0.26378223495702008</v>
+        <v>0.26302857142857144</v>
       </c>
       <c r="J2" s="6">
         <v>400</v>
@@ -4809,7 +5111,7 @@
       <c r="D4" s="8">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="15">
         <v>44.53</v>
       </c>
       <c r="F4">
@@ -4819,11 +5121,11 @@
         <v>0.16</v>
       </c>
       <c r="H4">
-        <v>331</v>
-      </c>
-      <c r="I4" s="14">
+        <v>332</v>
+      </c>
+      <c r="I4" s="11">
         <f>E4/H4</f>
-        <v>0.13453172205438066</v>
+        <v>0.1341265060240964</v>
       </c>
       <c r="J4">
         <v>400</v>
@@ -4869,7 +5171,7 @@
       <c r="D5" s="8">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="15">
         <v>28.54</v>
       </c>
       <c r="F5">
@@ -4879,11 +5181,11 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H5">
-        <v>322</v>
-      </c>
-      <c r="I5" s="14">
-        <f t="shared" ref="I5:I31" si="0">E5/H5</f>
-        <v>8.8633540372670808E-2</v>
+        <v>323</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" ref="I5:I41" si="0">E5/H5</f>
+        <v>8.8359133126934983E-2</v>
       </c>
       <c r="J5">
         <v>400</v>
@@ -4929,7 +5231,7 @@
       <c r="D6" s="8">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="15">
         <v>22.69</v>
       </c>
       <c r="F6">
@@ -4939,11 +5241,11 @@
         <v>0.39</v>
       </c>
       <c r="H6">
-        <v>313</v>
-      </c>
-      <c r="I6" s="14">
+        <v>314</v>
+      </c>
+      <c r="I6" s="11">
         <f t="shared" si="0"/>
-        <v>7.2492012779552722E-2</v>
+        <v>7.2261146496815296E-2</v>
       </c>
       <c r="J6">
         <v>400</v>
@@ -4989,7 +5291,7 @@
       <c r="D7" s="8">
         <v>5.3100000000000001E-2</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="15">
         <v>18.71</v>
       </c>
       <c r="F7">
@@ -4999,11 +5301,11 @@
         <v>0.46</v>
       </c>
       <c r="H7">
-        <v>304</v>
-      </c>
-      <c r="I7" s="14">
+        <v>305</v>
+      </c>
+      <c r="I7" s="11">
         <f t="shared" si="0"/>
-        <v>6.1546052631578953E-2</v>
+        <v>6.1344262295081969E-2</v>
       </c>
       <c r="J7">
         <v>400</v>
@@ -5049,7 +5351,7 @@
       <c r="D8" s="9">
         <v>9.5299999999999996E-2</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="16">
         <v>10.74</v>
       </c>
       <c r="F8" s="3">
@@ -5059,11 +5361,11 @@
         <v>1.6</v>
       </c>
       <c r="H8" s="3">
-        <v>229</v>
-      </c>
-      <c r="I8" s="17">
+        <v>230</v>
+      </c>
+      <c r="I8" s="13">
         <f t="shared" si="0"/>
-        <v>4.6899563318777295E-2</v>
+        <v>4.6695652173913048E-2</v>
       </c>
       <c r="J8" s="3">
         <v>400</v>
@@ -5097,33 +5399,33 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="11">
-        <v>50</v>
-      </c>
-      <c r="C9" s="18">
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="8">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="15">
         <v>43.43</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9">
         <v>1.06</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9">
         <v>0.18</v>
       </c>
-      <c r="H9" s="16">
-        <v>338</v>
-      </c>
-      <c r="I9" s="14">
+      <c r="H9">
+        <v>339</v>
+      </c>
+      <c r="I9" s="11">
         <f t="shared" si="0"/>
-        <v>0.12849112426035503</v>
+        <v>0.12811209439528023</v>
       </c>
       <c r="J9">
         <v>400</v>
@@ -5157,33 +5459,33 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10">
         <v>33</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="8">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="8">
         <v>3.9300000000000002E-2</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="15">
         <v>30.45</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10">
         <v>1.06</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10">
         <v>0.27</v>
       </c>
-      <c r="H10" s="12">
-        <v>326</v>
-      </c>
-      <c r="I10" s="14">
+      <c r="H10">
+        <v>327</v>
+      </c>
+      <c r="I10" s="11">
         <f t="shared" si="0"/>
-        <v>9.3404907975460125E-2</v>
+        <v>9.3119266055045863E-2</v>
       </c>
       <c r="J10">
         <v>400</v>
@@ -5217,33 +5519,33 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11">
         <v>25</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="8">
         <v>7.1800000000000003E-2</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="8">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="15">
         <v>23.47</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11">
         <v>1.06</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11">
         <v>0.36</v>
       </c>
-      <c r="H11" s="12">
-        <v>313</v>
-      </c>
-      <c r="I11" s="14">
+      <c r="H11">
+        <v>314</v>
+      </c>
+      <c r="I11" s="11">
         <f t="shared" si="0"/>
-        <v>7.4984025559105424E-2</v>
+        <v>7.4745222929936309E-2</v>
       </c>
       <c r="J11">
         <v>400</v>
@@ -5277,33 +5579,33 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12">
         <v>20</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="8">
         <v>8.7400000000000005E-2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="8">
         <v>5.1200000000000002E-2</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="15">
         <v>19.18</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12">
         <v>1.07</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12">
         <v>0.62</v>
       </c>
-      <c r="H12" s="12">
-        <v>306</v>
-      </c>
-      <c r="I12" s="14">
+      <c r="H12">
+        <v>307</v>
+      </c>
+      <c r="I12" s="11">
         <f t="shared" si="0"/>
-        <v>6.2679738562091497E-2</v>
+        <v>6.2475570032573292E-2</v>
       </c>
       <c r="J12">
         <v>400</v>
@@ -5337,33 +5639,33 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="9">
         <v>0.21340000000000001</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="9">
         <v>0.10340000000000001</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="16">
         <v>11.16</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="3">
         <v>1.01</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="3">
         <v>1.1200000000000001</v>
       </c>
-      <c r="H13" s="21">
-        <v>252</v>
-      </c>
-      <c r="I13" s="17">
+      <c r="H13" s="3">
+        <v>253</v>
+      </c>
+      <c r="I13" s="13">
         <f t="shared" si="0"/>
-        <v>4.4285714285714289E-2</v>
+        <v>4.4110671936758897E-2</v>
       </c>
       <c r="J13" s="3">
         <v>400</v>
@@ -5397,33 +5699,33 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14">
         <v>90</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="8">
         <v>8.5099999999999995E-2</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="8">
         <v>5.2200000000000003E-2</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="15">
         <v>110.15</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14">
         <v>1.06</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14">
         <v>0.11</v>
       </c>
-      <c r="H14" s="16">
-        <v>296</v>
-      </c>
-      <c r="I14" s="24">
+      <c r="H14">
+        <v>297</v>
+      </c>
+      <c r="I14" s="11">
         <f t="shared" si="0"/>
-        <v>0.37212837837837842</v>
+        <v>0.37087542087542091</v>
       </c>
       <c r="J14">
         <v>400</v>
@@ -5457,33 +5759,33 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>80</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="8">
         <v>0.1047</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="8">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="15">
         <v>89.53</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15">
         <v>1.06</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15">
         <v>0.11</v>
       </c>
-      <c r="H15" s="16">
-        <v>290</v>
-      </c>
-      <c r="I15" s="24">
+      <c r="H15">
+        <v>291</v>
+      </c>
+      <c r="I15" s="11">
         <f t="shared" si="0"/>
-        <v>0.30872413793103448</v>
+        <v>0.30766323024054981</v>
       </c>
       <c r="J15">
         <v>400</v>
@@ -5517,33 +5819,33 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16">
         <v>70</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="8">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="8">
         <v>4.36E-2</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="15">
         <v>73.28</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16">
         <v>1.06</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16">
         <v>0.11</v>
       </c>
-      <c r="H16" s="16">
-        <v>299</v>
-      </c>
-      <c r="I16" s="24">
+      <c r="H16">
+        <v>300</v>
+      </c>
+      <c r="I16" s="11">
         <f t="shared" si="0"/>
-        <v>0.24508361204013379</v>
+        <v>0.24426666666666666</v>
       </c>
       <c r="J16">
         <v>400</v>
@@ -5577,33 +5879,33 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17">
         <v>60</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="8">
         <v>8.5099999999999995E-2</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="8">
         <v>5.0900000000000001E-2</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="15">
         <v>65.94</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17">
         <v>1.06</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17">
         <v>0.15</v>
       </c>
-      <c r="H17" s="16">
-        <v>291</v>
-      </c>
-      <c r="I17" s="24">
+      <c r="H17">
+        <v>292</v>
+      </c>
+      <c r="I17" s="11">
         <f t="shared" si="0"/>
-        <v>0.22659793814432988</v>
+        <v>0.22582191780821917</v>
       </c>
       <c r="J17">
         <v>400</v>
@@ -5637,33 +5939,33 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="11">
-        <v>50</v>
-      </c>
-      <c r="C18" s="18">
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18" s="8">
         <v>9.7900000000000001E-2</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="8">
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="15">
         <v>54.77</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18">
         <v>1.08</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18">
         <v>0.19</v>
       </c>
-      <c r="H18" s="16">
-        <v>271</v>
-      </c>
-      <c r="I18" s="24">
+      <c r="H18">
+        <v>272</v>
+      </c>
+      <c r="I18" s="11">
         <f t="shared" si="0"/>
-        <v>0.20210332103321035</v>
+        <v>0.20136029411764708</v>
       </c>
       <c r="J18">
         <v>400</v>
@@ -5697,33 +5999,33 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19">
         <v>40</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="8">
         <v>9.64E-2</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="8">
         <v>5.8599999999999999E-2</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="15">
         <v>43.44</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19">
         <v>1.08</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19">
         <v>0.23</v>
       </c>
-      <c r="H19" s="16">
-        <v>270</v>
-      </c>
-      <c r="I19" s="24">
+      <c r="H19">
+        <v>271</v>
+      </c>
+      <c r="I19" s="11">
         <f t="shared" si="0"/>
-        <v>0.16088888888888889</v>
+        <v>0.16029520295202951</v>
       </c>
       <c r="J19">
         <v>400</v>
@@ -5757,33 +6059,33 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20">
         <v>30</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="8">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="8">
         <v>5.2600000000000001E-2</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="15">
         <v>30.46</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1.08</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20">
         <v>0.3</v>
       </c>
-      <c r="H20" s="12">
-        <v>277</v>
-      </c>
-      <c r="I20" s="24">
+      <c r="H20">
+        <v>278</v>
+      </c>
+      <c r="I20" s="11">
         <f t="shared" si="0"/>
-        <v>0.10996389891696751</v>
+        <v>0.109568345323741</v>
       </c>
       <c r="J20">
         <v>400</v>
@@ -5817,33 +6119,33 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="8">
         <v>0.1162</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="8">
         <v>6.7599999999999993E-2</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="15">
         <v>20.5</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <v>1.08</v>
       </c>
-      <c r="G21" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H21" s="12">
-        <v>247</v>
-      </c>
-      <c r="I21" s="24">
+      <c r="G21">
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <v>248</v>
+      </c>
+      <c r="I21" s="11">
         <f t="shared" si="0"/>
-        <v>8.2995951417004055E-2</v>
+        <v>8.2661290322580641E-2</v>
       </c>
       <c r="J21">
         <v>400</v>
@@ -5877,10 +6179,10 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="3">
         <v>10</v>
       </c>
       <c r="C22" s="3">
@@ -5889,21 +6191,21 @@
       <c r="D22" s="3">
         <v>0.1009</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="16">
         <v>10.83</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="3">
         <v>1.18</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="3">
         <v>0.62</v>
       </c>
-      <c r="H22" s="21">
-        <v>195</v>
-      </c>
-      <c r="I22" s="25">
+      <c r="H22" s="3">
+        <v>196</v>
+      </c>
+      <c r="I22" s="13">
         <f t="shared" si="0"/>
-        <v>5.5538461538461537E-2</v>
+        <v>5.525510204081633E-2</v>
       </c>
       <c r="J22" s="3">
         <v>400</v>
@@ -5937,33 +6239,33 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23">
         <v>90</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="8">
         <v>0.12809999999999999</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="8">
         <v>7.2900000000000006E-2</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="15">
         <v>150.76</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>0.88</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23">
         <v>0.13</v>
       </c>
-      <c r="H23" s="16">
-        <v>176</v>
-      </c>
-      <c r="I23" s="24">
+      <c r="H23">
+        <v>177</v>
+      </c>
+      <c r="I23" s="11">
         <f t="shared" si="0"/>
-        <v>0.85659090909090907</v>
+        <v>0.85175141242937846</v>
       </c>
       <c r="J23">
         <v>400</v>
@@ -5989,44 +6291,44 @@
       <c r="Q23" t="s">
         <v>17</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23">
         <v>4</v>
       </c>
       <c r="T23" t="s">
         <v>122</v>
       </c>
-      <c r="U23" s="33" t="s">
+      <c r="U23" s="20" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24">
         <v>80</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="8">
         <v>0.1085</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="8">
         <v>6.1899999999999997E-2</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="15">
         <v>125.29</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>1.06</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24">
         <v>0.17</v>
       </c>
-      <c r="H24" s="16">
-        <v>176</v>
-      </c>
-      <c r="I24" s="24">
+      <c r="H24">
+        <v>177</v>
+      </c>
+      <c r="I24" s="11">
         <f t="shared" si="0"/>
-        <v>0.71187500000000004</v>
+        <v>0.7078531073446328</v>
       </c>
       <c r="J24">
         <v>400</v>
@@ -6063,33 +6365,33 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25">
         <v>70</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="8">
         <v>0.11269999999999999</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="8">
         <v>6.3200000000000006E-2</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="15">
         <v>103.57</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25">
         <v>1.06</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25">
         <v>0.17</v>
       </c>
-      <c r="H25" s="16">
-        <v>171</v>
-      </c>
-      <c r="I25" s="24">
+      <c r="H25">
+        <v>172</v>
+      </c>
+      <c r="I25" s="11">
         <f t="shared" si="0"/>
-        <v>0.60567251461988303</v>
+        <v>0.60215116279069758</v>
       </c>
       <c r="J25">
         <v>400</v>
@@ -6123,33 +6425,33 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26">
         <v>60</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="8">
         <v>0.12429999999999999</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="8">
         <v>7.0900000000000005E-2</v>
       </c>
-      <c r="E26" s="28">
+      <c r="E26" s="15">
         <v>82.77</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>1.06</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26">
         <v>0.17</v>
       </c>
-      <c r="H26" s="16">
-        <v>175</v>
-      </c>
-      <c r="I26" s="24">
+      <c r="H26">
+        <v>176</v>
+      </c>
+      <c r="I26" s="11">
         <f t="shared" si="0"/>
-        <v>0.47297142857142854</v>
+        <v>0.4702840909090909</v>
       </c>
       <c r="J26">
         <v>400</v>
@@ -6183,33 +6485,33 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="11">
-        <v>50</v>
-      </c>
-      <c r="C27" s="18">
+      <c r="B27">
+        <v>50</v>
+      </c>
+      <c r="C27" s="8">
         <v>0.1111</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="8">
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="15">
         <v>67.3</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>1.1399999999999999</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27">
         <v>0.19</v>
       </c>
-      <c r="H27" s="16">
-        <v>172</v>
-      </c>
-      <c r="I27" s="24">
+      <c r="H27">
+        <v>173</v>
+      </c>
+      <c r="I27" s="11">
         <f t="shared" si="0"/>
-        <v>0.39127906976744187</v>
+        <v>0.38901734104046243</v>
       </c>
       <c r="J27">
         <v>400</v>
@@ -6243,33 +6545,33 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28">
         <v>40</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="8">
         <v>9.4899999999999998E-2</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="8">
         <v>5.6500000000000002E-2</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="15">
         <v>49.68</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>1.23</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28">
         <v>0.22</v>
       </c>
-      <c r="H28" s="16">
-        <v>163</v>
-      </c>
-      <c r="I28" s="24">
+      <c r="H28">
+        <v>164</v>
+      </c>
+      <c r="I28" s="11">
         <f t="shared" si="0"/>
-        <v>0.3047852760736196</v>
+        <v>0.30292682926829267</v>
       </c>
       <c r="J28">
         <v>400</v>
@@ -6303,33 +6605,33 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29">
         <v>30</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="8">
         <v>0.106</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="8">
         <v>6.2399999999999997E-2</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="15">
         <v>35.69</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29">
         <v>1.05</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29">
         <v>0.39</v>
       </c>
-      <c r="H29" s="16">
-        <v>166</v>
-      </c>
-      <c r="I29" s="24">
+      <c r="H29">
+        <v>167</v>
+      </c>
+      <c r="I29" s="11">
         <f t="shared" si="0"/>
-        <v>0.215</v>
+        <v>0.21371257485029937</v>
       </c>
       <c r="J29">
         <v>400</v>
@@ -6363,33 +6665,33 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30">
         <v>20</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="8">
         <v>0.10100000000000001</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="8">
         <v>6.2600000000000003E-2</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="15">
         <v>21.34</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30">
         <v>1.01</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30">
         <v>0.7</v>
       </c>
-      <c r="H30" s="16">
-        <v>161</v>
-      </c>
-      <c r="I30" s="24">
+      <c r="H30">
+        <v>162</v>
+      </c>
+      <c r="I30" s="11">
         <f t="shared" si="0"/>
-        <v>0.13254658385093168</v>
+        <v>0.1317283950617284</v>
       </c>
       <c r="J30">
         <v>400</v>
@@ -6423,10 +6725,10 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="3">
         <v>10</v>
       </c>
       <c r="C31" s="3">
@@ -6435,21 +6737,21 @@
       <c r="D31" s="3">
         <v>9.3899999999999997E-2</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="16">
         <v>10.29</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="3">
         <v>1.01</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="3">
         <v>1.64</v>
       </c>
-      <c r="H31" s="21">
-        <v>139</v>
-      </c>
-      <c r="I31" s="25">
+      <c r="H31" s="3">
+        <v>140</v>
+      </c>
+      <c r="I31" s="13">
         <f t="shared" si="0"/>
-        <v>7.4028776978417254E-2</v>
+        <v>7.3499999999999996E-2</v>
       </c>
       <c r="J31" s="3">
         <v>400</v>
@@ -6481,6 +6783,670 @@
       <c r="T31" t="s">
         <v>122</v>
       </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="24">
+        <v>90</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.12130000000000001</v>
+      </c>
+      <c r="D32" s="8">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="E32" s="30">
+        <v>158</v>
+      </c>
+      <c r="F32">
+        <v>1.25</v>
+      </c>
+      <c r="G32">
+        <v>0.09</v>
+      </c>
+      <c r="H32" s="24">
+        <v>189</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="0"/>
+        <v>0.83597883597883593</v>
+      </c>
+      <c r="J32">
+        <v>400</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+      <c r="O32" t="s">
+        <v>108</v>
+      </c>
+      <c r="P32" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>14</v>
+      </c>
+      <c r="R32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="24">
+        <v>80</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.1308</v>
+      </c>
+      <c r="D33" s="8">
+        <v>8.14E-2</v>
+      </c>
+      <c r="E33" s="30">
+        <v>119.32</v>
+      </c>
+      <c r="F33">
+        <v>1.06</v>
+      </c>
+      <c r="G33">
+        <v>0.09</v>
+      </c>
+      <c r="H33" s="24">
+        <v>185</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="0"/>
+        <v>0.64497297297297296</v>
+      </c>
+      <c r="J33">
+        <v>400</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33" t="s">
+        <v>108</v>
+      </c>
+      <c r="P33" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>14</v>
+      </c>
+      <c r="R33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="24">
+        <v>70</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="D34" s="8">
+        <v>7.4899999999999994E-2</v>
+      </c>
+      <c r="E34" s="30">
+        <v>97.72</v>
+      </c>
+      <c r="F34">
+        <v>1.06</v>
+      </c>
+      <c r="G34">
+        <v>0.11</v>
+      </c>
+      <c r="H34" s="24">
+        <v>183</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="0"/>
+        <v>0.53398907103825133</v>
+      </c>
+      <c r="J34">
+        <v>400</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+      <c r="O34" t="s">
+        <v>108</v>
+      </c>
+      <c r="P34" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>14</v>
+      </c>
+      <c r="R34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="24">
+        <v>60</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.1636</v>
+      </c>
+      <c r="D35" s="8">
+        <v>9.1899999999999996E-2</v>
+      </c>
+      <c r="E35" s="30">
+        <v>72.81</v>
+      </c>
+      <c r="F35">
+        <v>1.06</v>
+      </c>
+      <c r="G35">
+        <v>0.13</v>
+      </c>
+      <c r="H35" s="24">
+        <v>185</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="0"/>
+        <v>0.39356756756756756</v>
+      </c>
+      <c r="J35">
+        <v>400</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <v>4</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+      <c r="O35" t="s">
+        <v>108</v>
+      </c>
+      <c r="P35" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="24">
+        <v>50</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="D36" s="8">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="E36" s="30">
+        <v>56.88</v>
+      </c>
+      <c r="F36">
+        <v>1.06</v>
+      </c>
+      <c r="G36">
+        <v>0.21</v>
+      </c>
+      <c r="H36" s="24">
+        <v>178</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" si="0"/>
+        <v>0.31955056179775282</v>
+      </c>
+      <c r="J36">
+        <v>400</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>4</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="N36">
+        <v>3</v>
+      </c>
+      <c r="O36" t="s">
+        <v>108</v>
+      </c>
+      <c r="P36" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>14</v>
+      </c>
+      <c r="R36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="24">
+        <v>40</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.1348</v>
+      </c>
+      <c r="D37" s="8">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="E37" s="30">
+        <v>39.44</v>
+      </c>
+      <c r="F37">
+        <v>0.96</v>
+      </c>
+      <c r="G37">
+        <v>0.31</v>
+      </c>
+      <c r="H37" s="24">
+        <v>180</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="0"/>
+        <v>0.21911111111111109</v>
+      </c>
+      <c r="J37">
+        <v>400</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+      <c r="O37" t="s">
+        <v>108</v>
+      </c>
+      <c r="P37" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>14</v>
+      </c>
+      <c r="R37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="24">
+        <v>30</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.14019999999999999</v>
+      </c>
+      <c r="D38" s="8">
+        <v>9.1700000000000004E-2</v>
+      </c>
+      <c r="E38" s="30">
+        <v>27.93</v>
+      </c>
+      <c r="F38">
+        <v>0.96</v>
+      </c>
+      <c r="G38">
+        <v>0.39</v>
+      </c>
+      <c r="H38" s="24">
+        <v>181</v>
+      </c>
+      <c r="I38" s="11">
+        <f t="shared" si="0"/>
+        <v>0.15430939226519336</v>
+      </c>
+      <c r="J38">
+        <v>400</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+      <c r="O38" t="s">
+        <v>108</v>
+      </c>
+      <c r="P38" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>14</v>
+      </c>
+      <c r="R38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="24">
+        <v>20</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.16309999999999999</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0.1094</v>
+      </c>
+      <c r="E39" s="30">
+        <v>17.03</v>
+      </c>
+      <c r="F39">
+        <v>0.96</v>
+      </c>
+      <c r="G39">
+        <v>0.49</v>
+      </c>
+      <c r="H39" s="24">
+        <v>168</v>
+      </c>
+      <c r="I39" s="11">
+        <f t="shared" si="0"/>
+        <v>0.10136904761904762</v>
+      </c>
+      <c r="J39">
+        <v>400</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <v>4</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39" t="s">
+        <v>108</v>
+      </c>
+      <c r="P39" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>14</v>
+      </c>
+      <c r="R39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="31">
+        <v>10</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.19789999999999999</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.1376</v>
+      </c>
+      <c r="E40" s="32">
+        <v>9.9</v>
+      </c>
+      <c r="F40" s="33">
+        <v>0.96</v>
+      </c>
+      <c r="G40" s="33">
+        <v>0.71</v>
+      </c>
+      <c r="H40" s="31">
+        <v>161</v>
+      </c>
+      <c r="I40" s="13">
+        <f t="shared" si="0"/>
+        <v>6.1490683229813665E-2</v>
+      </c>
+      <c r="J40" s="3">
+        <v>400</v>
+      </c>
+      <c r="K40" s="3">
+        <v>4</v>
+      </c>
+      <c r="L40" s="3">
+        <v>4</v>
+      </c>
+      <c r="M40" s="3">
+        <v>3</v>
+      </c>
+      <c r="N40" s="3">
+        <v>3</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R40" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="24">
+        <v>90</v>
+      </c>
+      <c r="F41" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G41" s="34">
+        <v>0.09</v>
+      </c>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="24">
+        <v>80</v>
+      </c>
+      <c r="F42" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G42" s="34">
+        <v>0.11</v>
+      </c>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="24">
+        <v>70</v>
+      </c>
+      <c r="F43" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G43" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="24">
+        <v>60</v>
+      </c>
+      <c r="F44" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G44" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="24">
+        <v>50</v>
+      </c>
+      <c r="F45" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G45" s="34">
+        <v>0.19</v>
+      </c>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="24">
+        <v>40</v>
+      </c>
+      <c r="F46" s="34">
+        <v>1.06</v>
+      </c>
+      <c r="G46" s="34">
+        <v>0.24</v>
+      </c>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="24">
+        <v>30</v>
+      </c>
+      <c r="F47" s="34">
+        <v>1.27</v>
+      </c>
+      <c r="G47" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="24">
+        <v>20</v>
+      </c>
+      <c r="F48" s="34">
+        <v>1.27</v>
+      </c>
+      <c r="G48" s="34">
+        <v>0.39</v>
+      </c>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="31">
+        <v>10</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="36">
+        <v>1.45</v>
+      </c>
+      <c r="G49" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1048576" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hefty figs and presentation
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4C4147-2A95-466B-8C71-C9FD94462A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB04DEB-0E3F-4F54-B56D-DB7514F5B386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" activeTab="2" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="131">
   <si>
     <t>exact</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>may need to rerun if 70 doesn't converge, watch sparsity closesly</t>
+  </si>
+  <si>
+    <t>day 3</t>
   </si>
 </sst>
 </file>
@@ -4950,8 +4953,8 @@
   <dimension ref="A1:V76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6831,8 +6834,11 @@
       <c r="R32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -6888,8 +6894,11 @@
       <c r="R33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -6945,8 +6954,11 @@
       <c r="R34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -7002,8 +7014,11 @@
       <c r="R35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -7059,8 +7074,11 @@
       <c r="R36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -7116,8 +7134,11 @@
       <c r="R37">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -7173,8 +7194,11 @@
       <c r="R38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -7230,8 +7254,11 @@
       <c r="R39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
@@ -7287,8 +7314,11 @@
       <c r="R40" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T40" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -7344,8 +7374,11 @@
       <c r="R41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -7401,8 +7434,11 @@
       <c r="R42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -7458,8 +7494,11 @@
       <c r="R43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -7515,8 +7554,11 @@
       <c r="R44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -7572,8 +7614,11 @@
       <c r="R45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -7629,8 +7674,11 @@
       <c r="R46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -7686,8 +7734,11 @@
       <c r="R47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -7743,8 +7794,11 @@
       <c r="R48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
@@ -7800,14 +7854,17 @@
       <c r="R49" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H56">
         <f>SUM(H1:H49)</f>
         <v>11868</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D63">
         <v>50</v>
       </c>
@@ -7827,7 +7884,7 @@
         <v>0.1341265060240964</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D64">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
new plots and updates data
</commit_message>
<xml_diff>
--- a/post_processing/training_hp.xlsx
+++ b/post_processing/training_hp.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phillip\Documents\PhilRepo\gpr_ms_thesis\post_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F743F645-579F-4E53-A191-4C155E3CD16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256CF00-01A8-4E8D-A418-AEBF5F76FD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12504" activeTab="3" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{CD67D51D-A573-4111-BD5E-BD0B8ABCC759}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="train" sheetId="2" r:id="rId2"/>
     <sheet name="inference" sheetId="3" r:id="rId3"/>
     <sheet name="inference_better" sheetId="4" r:id="rId4"/>
+    <sheet name="sys_timing" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="138">
   <si>
     <t>exact</t>
   </si>
@@ -441,6 +442,18 @@
   </si>
   <si>
     <t>kmeans still took about 20 seconds before getting into the actual processing, not sure why this was</t>
+  </si>
+  <si>
+    <t>NOTE EVRYTHING HERE REALTES TO INFERENCE TIME. NOT TOTAL SYSTEM TIME. SEE OTHER SHEET FOR SYSTEM TIMING</t>
+  </si>
+  <si>
+    <t>sys Runtime</t>
+  </si>
+  <si>
+    <t>norm runtime</t>
+  </si>
+  <si>
+    <t>total pcds is taken from the inference_better sheet. A bash script was used to get the total system compute time. Norm runtime is sys runtime / total pcds</t>
   </si>
 </sst>
 </file>
@@ -451,7 +464,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,8 +488,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +533,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -546,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -580,10 +606,18 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8042,11 +8076,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6019AA57-D6F4-4382-85C6-FE786990F422}">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8060,7 +8094,7 @@
     <col min="18" max="18" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -8121,7 +8155,7 @@
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8184,7 +8218,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>131</v>
       </c>
@@ -8203,8 +8237,21 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q3" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -8264,7 +8311,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -8324,7 +8371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -8384,7 +8431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -8444,7 +8491,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -8504,7 +8551,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -8564,7 +8611,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -8624,7 +8671,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -8684,7 +8731,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -8744,7 +8791,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -8804,7 +8851,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8829,7 +8876,7 @@
       <c r="H14" s="7">
         <v>344</v>
       </c>
-      <c r="I14" s="35">
+      <c r="I14" s="34">
         <f t="shared" si="0"/>
         <v>0.23811046511627906</v>
       </c>
@@ -8864,7 +8911,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -8889,7 +8936,7 @@
       <c r="H15" s="7">
         <v>346</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="34">
         <f t="shared" si="0"/>
         <v>0.20835260115606938</v>
       </c>
@@ -8924,7 +8971,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -8949,7 +8996,7 @@
       <c r="H16" s="7">
         <v>340</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="34">
         <f t="shared" si="0"/>
         <v>0.18244117647058825</v>
       </c>
@@ -9009,7 +9056,7 @@
       <c r="H17" s="7">
         <v>342</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="34">
         <f t="shared" si="0"/>
         <v>0.15649122807017546</v>
       </c>
@@ -9072,7 +9119,7 @@
       <c r="H18" s="7">
         <v>335</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="34">
         <f t="shared" si="0"/>
         <v>0.12695522388059702</v>
       </c>
@@ -9132,7 +9179,7 @@
       <c r="H19" s="7">
         <v>323</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I19" s="34">
         <f t="shared" si="0"/>
         <v>0.11024767801857585</v>
       </c>
@@ -9192,7 +9239,7 @@
       <c r="H20" s="7">
         <v>314</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="34">
         <f t="shared" si="0"/>
         <v>8.4872611464968148E-2</v>
       </c>
@@ -9252,7 +9299,7 @@
       <c r="H21" s="7">
         <v>312</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="34">
         <f t="shared" si="0"/>
         <v>6.0256410256410257E-2</v>
       </c>
@@ -9294,10 +9341,10 @@
       <c r="B22" s="3">
         <v>10</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="33">
         <v>0.1618</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="33">
         <v>9.0300000000000005E-2</v>
       </c>
       <c r="E22" s="32">
@@ -9309,10 +9356,10 @@
       <c r="G22" s="3">
         <v>0.62</v>
       </c>
-      <c r="H22" s="34">
+      <c r="H22" s="33">
         <v>222</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I22" s="35">
         <f t="shared" si="0"/>
         <v>4.7387387387387382E-2</v>
       </c>
@@ -9372,7 +9419,7 @@
       <c r="H23" s="7">
         <v>348</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="34">
         <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
@@ -9433,7 +9480,7 @@
       <c r="H24" s="7">
         <v>344</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I24" s="34">
         <f t="shared" si="0"/>
         <v>0.20805232558139533</v>
       </c>
@@ -9496,7 +9543,7 @@
       <c r="H25" s="7">
         <v>344</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I25" s="34">
         <f t="shared" si="0"/>
         <v>0.18063953488372092</v>
       </c>
@@ -9556,7 +9603,7 @@
       <c r="H26" s="7">
         <v>342</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="34">
         <f t="shared" si="0"/>
         <v>0.15485380116959063</v>
       </c>
@@ -9616,7 +9663,7 @@
       <c r="H27" s="7">
         <v>339</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="34">
         <f t="shared" si="0"/>
         <v>0.13168141592920354</v>
       </c>
@@ -9676,7 +9723,7 @@
       <c r="H28" s="7">
         <v>330</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="34">
         <f t="shared" si="0"/>
         <v>0.10803030303030303</v>
       </c>
@@ -9736,7 +9783,7 @@
       <c r="H29" s="7">
         <v>317</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="34">
         <f t="shared" si="0"/>
         <v>8.293375394321767E-2</v>
       </c>
@@ -9796,7 +9843,7 @@
       <c r="H30" s="7">
         <v>317</v>
       </c>
-      <c r="I30" s="35">
+      <c r="I30" s="34">
         <f t="shared" si="0"/>
         <v>6.1104100946372246E-2</v>
       </c>
@@ -9838,10 +9885,10 @@
       <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="33">
         <v>0.17780000000000001</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="33">
         <v>9.5200000000000007E-2</v>
       </c>
       <c r="E31" s="32">
@@ -9853,10 +9900,10 @@
       <c r="G31" s="3">
         <v>1.64</v>
       </c>
-      <c r="H31" s="34">
+      <c r="H31" s="33">
         <v>234</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="35">
         <f t="shared" si="0"/>
         <v>4.4487179487179486E-2</v>
       </c>
@@ -9913,10 +9960,10 @@
       <c r="G32">
         <v>0.09</v>
       </c>
-      <c r="H32" s="33">
+      <c r="H32" s="7">
         <v>367</v>
       </c>
-      <c r="I32" s="35">
+      <c r="I32" s="34">
         <f>E32/H32</f>
         <v>0.24321525885558584</v>
       </c>
@@ -9973,10 +10020,10 @@
       <c r="G33">
         <v>0.09</v>
       </c>
-      <c r="H33" s="33">
+      <c r="H33" s="7">
         <v>343</v>
       </c>
-      <c r="I33" s="35">
+      <c r="I33" s="34">
         <f t="shared" si="0"/>
         <v>0.21323615160349854</v>
       </c>
@@ -10036,7 +10083,7 @@
       <c r="H34" s="7">
         <v>350</v>
       </c>
-      <c r="I34" s="35">
+      <c r="I34" s="34">
         <f t="shared" si="0"/>
         <v>0.17265714285714287</v>
       </c>
@@ -10096,7 +10143,7 @@
       <c r="H35" s="7">
         <v>318</v>
       </c>
-      <c r="I35" s="35">
+      <c r="I35" s="34">
         <f t="shared" si="0"/>
         <v>0.16059748427672957</v>
       </c>
@@ -10156,7 +10203,7 @@
       <c r="H36" s="7">
         <v>343</v>
       </c>
-      <c r="I36" s="35">
+      <c r="I36" s="34">
         <f t="shared" si="0"/>
         <v>0.12565597667638484</v>
       </c>
@@ -10219,7 +10266,7 @@
       <c r="H37" s="7">
         <v>302</v>
       </c>
-      <c r="I37" s="35">
+      <c r="I37" s="34">
         <f t="shared" si="0"/>
         <v>0.10827814569536424</v>
       </c>
@@ -10279,7 +10326,7 @@
       <c r="H38" s="7">
         <v>307</v>
       </c>
-      <c r="I38" s="35">
+      <c r="I38" s="34">
         <f t="shared" si="0"/>
         <v>8.3811074918566777E-2</v>
       </c>
@@ -10339,7 +10386,7 @@
       <c r="H39" s="7">
         <v>166</v>
       </c>
-      <c r="I39" s="35">
+      <c r="I39" s="34">
         <f t="shared" si="0"/>
         <v>9.9036144578313265E-2</v>
       </c>
@@ -10396,10 +10443,10 @@
       <c r="G40" s="27">
         <v>0.71</v>
       </c>
-      <c r="H40" s="34">
+      <c r="H40" s="33">
         <v>167</v>
       </c>
-      <c r="I40" s="36">
+      <c r="I40" s="35">
         <f t="shared" si="0"/>
         <v>6.1137724550898206E-2</v>
       </c>
@@ -11135,4 +11182,895 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BC7736-ACF7-46C3-BBEF-778A611A80A4}">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100</v>
+      </c>
+      <c r="C2" s="39">
+        <v>186.04300000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>350</v>
+      </c>
+      <c r="E2" s="13">
+        <f>C2/D2</f>
+        <v>0.53155142857142856</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3" s="40">
+        <v>90.662468512000004</v>
+      </c>
+      <c r="D3" s="42">
+        <v>332</v>
+      </c>
+      <c r="E3" s="44">
+        <f t="shared" ref="E3:E48" si="0">C3/D3</f>
+        <v>0.27307972443373496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4" s="40">
+        <v>74.905509205000001</v>
+      </c>
+      <c r="D4" s="42">
+        <v>323</v>
+      </c>
+      <c r="E4" s="44">
+        <f t="shared" si="0"/>
+        <v>0.23190560125386997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" s="40">
+        <v>65.869185521000006</v>
+      </c>
+      <c r="D5" s="42">
+        <v>314</v>
+      </c>
+      <c r="E5" s="44">
+        <f t="shared" si="0"/>
+        <v>0.20977447618152867</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6" s="40">
+        <v>61.518089058000001</v>
+      </c>
+      <c r="D6" s="42">
+        <v>305</v>
+      </c>
+      <c r="E6" s="44">
+        <f t="shared" si="0"/>
+        <v>0.20169865264918033</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="41">
+        <v>45.804592939999999</v>
+      </c>
+      <c r="D7" s="43">
+        <v>230</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.19915040408695653</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8" s="40">
+        <v>90.653508251000005</v>
+      </c>
+      <c r="D8" s="42">
+        <v>339</v>
+      </c>
+      <c r="E8" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26741447861651918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9" s="40">
+        <v>74.687405350000006</v>
+      </c>
+      <c r="D9" s="42">
+        <v>327</v>
+      </c>
+      <c r="E9" s="44">
+        <f t="shared" si="0"/>
+        <v>0.22840185122324161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" s="40">
+        <v>67.139143765</v>
+      </c>
+      <c r="D10" s="42">
+        <v>314</v>
+      </c>
+      <c r="E10" s="44">
+        <f t="shared" si="0"/>
+        <v>0.21381892918789808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" s="40">
+        <v>61.912639601000002</v>
+      </c>
+      <c r="D11" s="42">
+        <v>307</v>
+      </c>
+      <c r="E11" s="44">
+        <f t="shared" si="0"/>
+        <v>0.20166983583387624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="41">
+        <v>49.501301941999998</v>
+      </c>
+      <c r="D12" s="43">
+        <v>253</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.19565731992885374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>90</v>
+      </c>
+      <c r="C13" s="40">
+        <v>130.70322751</v>
+      </c>
+      <c r="D13" s="42">
+        <v>344</v>
+      </c>
+      <c r="E13" s="44">
+        <f t="shared" si="0"/>
+        <v>0.37995124276162789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>80</v>
+      </c>
+      <c r="C14" s="40">
+        <v>121.208269298</v>
+      </c>
+      <c r="D14" s="42">
+        <v>346</v>
+      </c>
+      <c r="E14" s="44">
+        <f t="shared" si="0"/>
+        <v>0.35031291704624279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="C15" s="40">
+        <v>109.732610343</v>
+      </c>
+      <c r="D15" s="42">
+        <v>340</v>
+      </c>
+      <c r="E15" s="44">
+        <f t="shared" si="0"/>
+        <v>0.32274297159705884</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16" s="40">
+        <v>101.47397178999999</v>
+      </c>
+      <c r="D16" s="42">
+        <v>342</v>
+      </c>
+      <c r="E16" s="44">
+        <f t="shared" si="0"/>
+        <v>0.29670751985380117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17" s="40">
+        <v>89.924309426999997</v>
+      </c>
+      <c r="D17" s="42">
+        <v>335</v>
+      </c>
+      <c r="E17" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26843077440895524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18" s="40">
+        <v>79.580939916000005</v>
+      </c>
+      <c r="D18" s="42">
+        <v>323</v>
+      </c>
+      <c r="E18" s="44">
+        <f t="shared" si="0"/>
+        <v>0.24638061893498453</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19" s="40">
+        <v>70.255497257000002</v>
+      </c>
+      <c r="D19" s="42">
+        <v>314</v>
+      </c>
+      <c r="E19" s="44">
+        <f t="shared" si="0"/>
+        <v>0.22374362183757962</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" s="40">
+        <v>63.251994138999997</v>
+      </c>
+      <c r="D20" s="42">
+        <v>312</v>
+      </c>
+      <c r="E20" s="44">
+        <f t="shared" si="0"/>
+        <v>0.20273075044551281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+      <c r="C21" s="41">
+        <v>45.235274138000001</v>
+      </c>
+      <c r="D21" s="43">
+        <v>222</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.20376249611711711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>90</v>
+      </c>
+      <c r="C22" s="40">
+        <v>188.18063536299999</v>
+      </c>
+      <c r="D22" s="42">
+        <v>348</v>
+      </c>
+      <c r="E22" s="44">
+        <f t="shared" si="0"/>
+        <v>0.54074895219252872</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>80</v>
+      </c>
+      <c r="C23" s="40">
+        <v>173.20436882600001</v>
+      </c>
+      <c r="D23" s="42">
+        <v>344</v>
+      </c>
+      <c r="E23" s="44">
+        <f t="shared" si="0"/>
+        <v>0.50350107216860462</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>70</v>
+      </c>
+      <c r="C24" s="40">
+        <v>156.276430804</v>
+      </c>
+      <c r="D24" s="42">
+        <v>344</v>
+      </c>
+      <c r="E24" s="44">
+        <f t="shared" si="0"/>
+        <v>0.45429195001162792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25" s="40">
+        <v>141.025924229</v>
+      </c>
+      <c r="D25" s="42">
+        <v>342</v>
+      </c>
+      <c r="E25" s="44">
+        <f t="shared" si="0"/>
+        <v>0.41235650359356724</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26" s="40">
+        <v>123.616888495</v>
+      </c>
+      <c r="D26" s="42">
+        <v>339</v>
+      </c>
+      <c r="E26" s="44">
+        <f t="shared" si="0"/>
+        <v>0.36465158848082596</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>40</v>
+      </c>
+      <c r="C27" s="40">
+        <v>107.442286279</v>
+      </c>
+      <c r="D27" s="42">
+        <v>330</v>
+      </c>
+      <c r="E27" s="44">
+        <f t="shared" si="0"/>
+        <v>0.32558268569393939</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28" s="40">
+        <v>91.694261588000003</v>
+      </c>
+      <c r="D28" s="42">
+        <v>317</v>
+      </c>
+      <c r="E28" s="44">
+        <f t="shared" si="0"/>
+        <v>0.28925634570347003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" s="40">
+        <v>77.847419880999993</v>
+      </c>
+      <c r="D29" s="42">
+        <v>317</v>
+      </c>
+      <c r="E29" s="44">
+        <f t="shared" si="0"/>
+        <v>0.24557545703785486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="3">
+        <v>10</v>
+      </c>
+      <c r="C30" s="41">
+        <v>53.844025615</v>
+      </c>
+      <c r="D30" s="43">
+        <v>234</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>0.23010267356837608</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>90</v>
+      </c>
+      <c r="C31" s="40">
+        <v>141.130154995</v>
+      </c>
+      <c r="D31" s="42">
+        <v>367</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" si="0"/>
+        <v>0.3845508310490463</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>80</v>
+      </c>
+      <c r="C32" s="40">
+        <v>123.52008198599999</v>
+      </c>
+      <c r="D32" s="42">
+        <v>343</v>
+      </c>
+      <c r="E32" s="44">
+        <f t="shared" si="0"/>
+        <v>0.36011685710204078</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>70</v>
+      </c>
+      <c r="C33" s="40">
+        <v>110.041769891</v>
+      </c>
+      <c r="D33" s="42">
+        <v>350</v>
+      </c>
+      <c r="E33" s="44">
+        <f t="shared" si="0"/>
+        <v>0.31440505683142855</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34" s="40">
+        <v>95.864095978999998</v>
+      </c>
+      <c r="D34" s="42">
+        <v>318</v>
+      </c>
+      <c r="E34" s="44">
+        <f t="shared" si="0"/>
+        <v>0.30145942131761005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35" s="40">
+        <v>90.182015382000003</v>
+      </c>
+      <c r="D35" s="42">
+        <v>343</v>
+      </c>
+      <c r="E35" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26292132764431486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>40</v>
+      </c>
+      <c r="C36" s="40">
+        <v>75.143122665000007</v>
+      </c>
+      <c r="D36" s="42">
+        <v>302</v>
+      </c>
+      <c r="E36" s="44">
+        <f t="shared" si="0"/>
+        <v>0.2488182869701987</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>30</v>
+      </c>
+      <c r="C37" s="40">
+        <v>70.190814381999999</v>
+      </c>
+      <c r="D37" s="42">
+        <v>307</v>
+      </c>
+      <c r="E37" s="44">
+        <f t="shared" si="0"/>
+        <v>0.22863457453420194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38" s="40">
+        <v>43.971239369000003</v>
+      </c>
+      <c r="D38" s="42">
+        <v>166</v>
+      </c>
+      <c r="E38" s="44">
+        <f t="shared" si="0"/>
+        <v>0.26488698415060241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="3">
+        <v>10</v>
+      </c>
+      <c r="C39" s="41">
+        <v>38.09240183</v>
+      </c>
+      <c r="D39" s="43">
+        <v>167</v>
+      </c>
+      <c r="E39" s="13">
+        <f t="shared" si="0"/>
+        <v>0.22809821455089821</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>90</v>
+      </c>
+      <c r="C40" s="40">
+        <v>134.83930686599999</v>
+      </c>
+      <c r="D40" s="42">
+        <v>353</v>
+      </c>
+      <c r="E40" s="44">
+        <f t="shared" si="0"/>
+        <v>0.38198103928045324</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>80</v>
+      </c>
+      <c r="C41" s="40">
+        <v>120.525108265</v>
+      </c>
+      <c r="D41" s="42">
+        <v>344</v>
+      </c>
+      <c r="E41" s="44">
+        <f t="shared" si="0"/>
+        <v>0.35036368681686048</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>70</v>
+      </c>
+      <c r="C42" s="40">
+        <v>111.766605306</v>
+      </c>
+      <c r="D42" s="42">
+        <v>344</v>
+      </c>
+      <c r="E42" s="44">
+        <f t="shared" si="0"/>
+        <v>0.32490292240116281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>60</v>
+      </c>
+      <c r="C43" s="40">
+        <v>101.095132189</v>
+      </c>
+      <c r="D43" s="42">
+        <v>340</v>
+      </c>
+      <c r="E43" s="44">
+        <f t="shared" si="0"/>
+        <v>0.2973386240852941</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>50</v>
+      </c>
+      <c r="C44" s="40">
+        <v>93.742689599000002</v>
+      </c>
+      <c r="D44" s="42">
+        <v>339</v>
+      </c>
+      <c r="E44" s="44">
+        <f t="shared" si="0"/>
+        <v>0.27652710796165192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>40</v>
+      </c>
+      <c r="C45" s="40">
+        <v>82.902528302999997</v>
+      </c>
+      <c r="D45" s="42">
+        <v>331</v>
+      </c>
+      <c r="E45" s="44">
+        <f t="shared" si="0"/>
+        <v>0.25046081058308156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46" s="40">
+        <v>73.374082428999998</v>
+      </c>
+      <c r="D46" s="42">
+        <v>321</v>
+      </c>
+      <c r="E46" s="44">
+        <f t="shared" si="0"/>
+        <v>0.22857969604049844</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47" s="40">
+        <v>61.238409093000001</v>
+      </c>
+      <c r="D47" s="42">
+        <v>303</v>
+      </c>
+      <c r="E47" s="44">
+        <f t="shared" si="0"/>
+        <v>0.2021069607029703</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3">
+        <v>10</v>
+      </c>
+      <c r="C48" s="41">
+        <v>48.135981633</v>
+      </c>
+      <c r="D48" s="43">
+        <v>236</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="0"/>
+        <v>0.20396602386864407</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C8:C12">
+    <sortCondition descending="1" ref="C8:C12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>